<commit_message>
Add loading leds from excel
</commit_message>
<xml_diff>
--- a/spreadsheets/prices.xlsx
+++ b/spreadsheets/prices.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E3A02A-6E62-CB48-AA0C-11C7BDA9A436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F78EAB-3827-5845-A174-05563CFE9B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Буквы" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="65">
   <si>
     <t>Высота</t>
   </si>
@@ -226,24 +226,6 @@
   </si>
   <si>
     <t xml:space="preserve">цена за шт </t>
-  </si>
-  <si>
-    <t>42р</t>
-  </si>
-  <si>
-    <t>39р</t>
-  </si>
-  <si>
-    <t>36р</t>
-  </si>
-  <si>
-    <t>28р</t>
-  </si>
-  <si>
-    <t>23р</t>
-  </si>
-  <si>
-    <t>20р</t>
   </si>
 </sst>
 </file>
@@ -690,7 +672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:BF51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="143" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="143" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
@@ -7163,8 +7145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C656B8B6-C519-B541-95A4-11671C167167}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7200,23 +7182,23 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>65</v>
+      <c r="A3" s="13">
+        <v>20</v>
+      </c>
+      <c r="B3" s="14">
+        <v>23</v>
+      </c>
+      <c r="C3" s="14">
+        <v>28</v>
+      </c>
+      <c r="D3" s="14">
+        <v>36</v>
+      </c>
+      <c r="E3" s="8">
+        <v>39</v>
+      </c>
+      <c r="F3" s="9">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add loading power supplies from excel
</commit_message>
<xml_diff>
--- a/spreadsheets/prices.xlsx
+++ b/spreadsheets/prices.xlsx
@@ -3,13 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F78EAB-3827-5845-A174-05563CFE9B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDD8D60-7EF8-9443-B977-CCB89D5B8324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Буквы" sheetId="1" r:id="rId1"/>
     <sheet name="Светодиоды" sheetId="2" r:id="rId2"/>
+    <sheet name="Блоки питания" sheetId="3" r:id="rId3"/>
+    <sheet name="Лицевая часть" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="104">
   <si>
     <t>Высота</t>
   </si>
@@ -226,13 +228,134 @@
   </si>
   <si>
     <t xml:space="preserve">цена за шт </t>
+  </si>
+  <si>
+    <t>30Вт/12В герметичный IP67</t>
+  </si>
+  <si>
+    <t>40Вт/12В герметичный IP67</t>
+  </si>
+  <si>
+    <t>60Вт/12В герметичный IP67</t>
+  </si>
+  <si>
+    <t>100Вт/12В герметичный IP67</t>
+  </si>
+  <si>
+    <t>150Вт/12В герметичный IP67</t>
+  </si>
+  <si>
+    <t>200Вт/12В герметичный IP67</t>
+  </si>
+  <si>
+    <t>300Вт/12В герметичный IP67</t>
+  </si>
+  <si>
+    <t>АЛЮМИНИЕВЫЕ КОМПОЗИТНЫЕ ПАНЕЛИ</t>
+  </si>
+  <si>
+    <t>АЛЮМИНИЕВЫЕ КОМПОЗИТНЫЕ ПАНЕЛИ ALTEC</t>
+  </si>
+  <si>
+    <t>3 мм/0,21 (1220мм х 4000мм)</t>
+  </si>
+  <si>
+    <t>3 мм/0,21 (1500мм х 4000мм)</t>
+  </si>
+  <si>
+    <t>АЛЮМИНИЕВЫЕ КОМПОЗИТНЫЕ ПАНЕЛИ TUBOND</t>
+  </si>
+  <si>
+    <t>АКРИЛОВЫЕ СТЁКЛА (ОРГСТЕКЛО)</t>
+  </si>
+  <si>
+    <t>Акрил прозрачный Acryma</t>
+  </si>
+  <si>
+    <t>6 мм прозрачный (2050мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>Акрил прозрачный Tucryl</t>
+  </si>
+  <si>
+    <t>1,5 мм прозрачный (2050мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>Акрил прозрачный Plexiglas</t>
+  </si>
+  <si>
+    <t>2 мм прозрачный (2050мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>3 мм прозрачный (2050мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>4 мм прозрачный (2050мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>5 мм прозрачный (2050мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>8 мм прозрачный (2050мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>10 мм прозрачный (2050мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>Акрил Plexiglas опал (молочный, КСП 30%)</t>
+  </si>
+  <si>
+    <t>2 мм опал (2050мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>3 мм опал (2050мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>4 мм опал (2050мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>5 мм опал (2050мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>6 мм опал (2050мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>8 мм опал (2050мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>10 мм опал (2050мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>Акрил Plexiglas (белый, КСП 78%)</t>
+  </si>
+  <si>
+    <t>2 мм белый КСП 78% (2050мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>Акрил Plexiglas (черный)</t>
+  </si>
+  <si>
+    <t>3 мм черный (2050мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>Акрил литой ALTUGLAS (Франция)</t>
+  </si>
+  <si>
+    <t>Акрил литой Altuglas цветной 3 мм 2030*3050мм</t>
+  </si>
+  <si>
+    <t>Акрил литой Altuglas "День-Ночь" 3 мм 2030*3050мм черно-белый</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;RUB&quot;_-;\-* #,##0.00\ &quot;RUB&quot;_-;_-* &quot;-&quot;??\ &quot;RUB&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0&quot;р.&quot;_-;\-* #,##0&quot;р.&quot;_-;_-* &quot;-&quot;&quot;р.&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,16 +371,81 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -351,11 +539,121 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -376,8 +674,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -385,13 +681,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="4" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7132,8 +7473,8 @@
       <c r="BF48" s="6"/>
     </row>
     <row r="51" spans="10:11" x14ac:dyDescent="0.2">
-      <c r="J51" s="10"/>
-      <c r="K51" s="10"/>
+      <c r="J51" s="8"/>
+      <c r="K51" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7145,59 +7486,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C656B8B6-C519-B541-95A4-11671C167167}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="A2" s="9">
         <v>0.3</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="9">
         <v>0.36</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="9">
         <v>0.72</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="10">
         <v>1.3</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="10">
         <v>1.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="13">
+      <c r="A3" s="14">
         <v>20</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="15">
         <v>23</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="15">
         <v>28</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="15">
         <v>36</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="16">
         <v>39</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="17">
         <v>42</v>
       </c>
     </row>
@@ -7207,4 +7548,372 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD60F4EA-15D0-9249-8547-308D4B03F532}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="13">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="13">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="13">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="13">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="13">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="13">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="13">
+        <v>2900</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F9A308-2B62-FE4B-9E81-C392D976D579}">
+  <dimension ref="A1:B39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="50.1640625" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="35" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="18"/>
+      <c r="B1" s="30"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="31"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="20"/>
+      <c r="B3" s="32"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="33"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="34">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="34">
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="33"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="34">
+        <v>1633</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="34">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="22"/>
+      <c r="B10" s="31"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="31"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="20"/>
+      <c r="B12" s="32"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="33"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="34">
+        <v>3274</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="33"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="34">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="33"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="34">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="34">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="34">
+        <v>2423</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="34">
+        <v>2980</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="34">
+        <v>3738</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="34">
+        <v>4697</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="34">
+        <v>5876</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="33"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="34">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="34">
+        <v>1886</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="34">
+        <v>2435</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="34">
+        <v>3308</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" s="34">
+        <v>3367</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" s="34">
+        <v>5312</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" s="34">
+        <v>6397</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" s="33"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B34" s="34">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" s="33"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B36" s="34">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="B37" s="33"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="B38" s="34">
+        <v>2414</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" s="34">
+        <v>3570</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add front and back calculation from excel
</commit_message>
<xml_diff>
--- a/spreadsheets/prices.xlsx
+++ b/spreadsheets/prices.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDD8D60-7EF8-9443-B977-CCB89D5B8324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B14E3F-7720-8B49-8238-18A7B2995528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Буквы" sheetId="1" r:id="rId1"/>
     <sheet name="Светодиоды" sheetId="2" r:id="rId2"/>
     <sheet name="Блоки питания" sheetId="3" r:id="rId3"/>
     <sheet name="Лицевая часть" sheetId="4" r:id="rId4"/>
+    <sheet name="Задник" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="123">
   <si>
     <t>Высота</t>
   </si>
@@ -345,6 +346,63 @@
   </si>
   <si>
     <t>Акрил литой Altuglas "День-Ночь" 3 мм 2030*3050мм черно-белый</t>
+  </si>
+  <si>
+    <t>ПВХ вспененный (SIMONA, ONGROFOAM, ANWILL, X-FOAM)</t>
+  </si>
+  <si>
+    <t>ПВХ вспененный X-FOAM-N (Китай), белый, плотность 0,45 гр/cм3</t>
+  </si>
+  <si>
+    <t>2 мм (2050мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>3 мм (2050мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>4 мм (2050мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>5 мм (2050мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>6 мм (2050мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>8 мм (2050мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>10 мм (2050мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>ПВХ вспененный Ongrofoam (Венгрия), (X-FOAM (HU)), белый, плотность 0,45 гр/м3</t>
+  </si>
+  <si>
+    <t>10 мм (2030мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>ПВХ вспененный Simona, (TUFOAM TR, DE), белый, плотность 0,45 гр/cм3</t>
+  </si>
+  <si>
+    <t>ПВХ вспененный Unext fresh, белый, плотность 0,5 гр/cм3</t>
+  </si>
+  <si>
+    <t>2 мм (2030мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>3 мм (2030мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>6 мм (2030мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>ПВХ вспененный ANWILL, Польша (TUFOAM PL), белый, плотность 0,55 гр/cм3</t>
+  </si>
+  <si>
+    <t>ПВХ цветной вспененный (SIMONA, ONGROFOAM)</t>
+  </si>
+  <si>
+    <t>3 мм Simona (1530мм х 3050мм)</t>
   </si>
 </sst>
 </file>
@@ -355,7 +413,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;RUB&quot;_-;\-* #,##0.00\ &quot;RUB&quot;_-;_-* &quot;-&quot;??\ &quot;RUB&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0&quot;р.&quot;_-;\-* #,##0&quot;р.&quot;_-;_-* &quot;-&quot;&quot;р.&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -406,6 +464,15 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -445,7 +512,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -648,12 +715,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -714,22 +807,39 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="4" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="4" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="5" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -7629,14 +7739,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F9A308-2B62-FE4B-9E81-C392D976D579}">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.1640625" customWidth="1"/>
-    <col min="2" max="2" width="13.5" style="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="35" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -7915,5 +8025,547 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15234C30-08B1-B740-A3C1-96E9D3AD5C80}">
+  <dimension ref="A1:B71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="74.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="37"/>
+      <c r="B1" s="42"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="43"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="38"/>
+      <c r="B3" s="44"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="39"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="40">
+        <v>454.55502009722426</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="40">
+        <v>611.12397146404589</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="40">
+        <v>723.92095793261637</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="40">
+        <v>774.42707127675249</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" s="40">
+        <v>1043.7930091121445</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="40">
+        <v>1262.6528336034007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" s="39"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="40">
+        <v>420.88427786780028</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="40">
+        <v>276.10008628127696</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="40">
+        <v>732.33864348997236</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="40">
+        <v>791.20351859256289</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="40">
+        <v>622.90873124434438</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" s="40">
+        <v>816.51549906353239</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" s="40">
+        <v>969.07049987886626</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="39"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="40">
+        <v>505.06113344136043</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" s="40">
+        <v>707.08558681790453</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="40">
+        <v>824.93318462088871</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" s="40">
+        <v>826.61672173235979</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" s="40">
+        <v>1431.006544750521</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" s="40">
+        <v>1633.0309981270652</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" s="39"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="B27" s="40">
+        <v>368.69462741219309</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28" s="40">
+        <v>456.23855720869557</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="B29" s="40">
+        <v>878.8063721879671</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" s="39"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31" s="40">
+        <v>260.94825227803614</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" s="40">
+        <v>572.40261790020838</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" s="40">
+        <v>572.40261790020838</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" s="40">
+        <v>883.85698352238046</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" s="40">
+        <v>715.50327237526039</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="40">
+        <v>993.28689576800866</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" s="40">
+        <v>1683.5371114712011</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="B38" s="39"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" s="40">
+        <v>791.26244239146456</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" s="40">
+        <v>721.83029093144319</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" s="40">
+        <v>1341.7790778425476</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="22"/>
+      <c r="B42" s="31"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" s="31"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="20"/>
+      <c r="B44" s="32"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B45" s="33"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" s="34">
+        <v>3274</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B47" s="33"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B48" s="34">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B49" s="33"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B50" s="34">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B51" s="34">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B52" s="34">
+        <v>2423</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B53" s="34">
+        <v>2980</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B54" s="34">
+        <v>3738</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B55" s="34">
+        <v>4697</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B56" s="34">
+        <v>5876</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B57" s="33"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="B58" s="34">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B59" s="34">
+        <v>1886</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B60" s="34">
+        <v>2435</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B61" s="34">
+        <v>3308</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B62" s="34">
+        <v>3367</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="B63" s="34">
+        <v>5312</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B64" s="34">
+        <v>6397</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B65" s="33"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B66" s="34">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B67" s="33"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B68" s="34">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="B69" s="33"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="B70" s="34">
+        <v>2414</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B71" s="34">
+        <v>3570</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add loading frame materials from excel
</commit_message>
<xml_diff>
--- a/spreadsheets/prices.xlsx
+++ b/spreadsheets/prices.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B14E3F-7720-8B49-8238-18A7B2995528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C26654-5889-7541-8DEF-353C0A7B2949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19740" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Буквы" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="Блоки питания" sheetId="3" r:id="rId3"/>
     <sheet name="Лицевая часть" sheetId="4" r:id="rId4"/>
     <sheet name="Задник" sheetId="5" r:id="rId5"/>
+    <sheet name="Каркас" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="132">
   <si>
     <t>Высота</t>
   </si>
@@ -403,6 +404,33 @@
   </si>
   <si>
     <t>3 мм Simona (1530мм х 3050мм)</t>
+  </si>
+  <si>
+    <t>Лист</t>
+  </si>
+  <si>
+    <t>Труба</t>
+  </si>
+  <si>
+    <t>Профильная металлическая труба</t>
+  </si>
+  <si>
+    <t>15х15</t>
+  </si>
+  <si>
+    <t>20х20</t>
+  </si>
+  <si>
+    <t>25х25</t>
+  </si>
+  <si>
+    <t>30х30</t>
+  </si>
+  <si>
+    <t>40х40</t>
+  </si>
+  <si>
+    <t>50х50</t>
   </si>
 </sst>
 </file>
@@ -413,7 +441,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;RUB&quot;_-;\-* #,##0.00\ &quot;RUB&quot;_-;_-* &quot;-&quot;??\ &quot;RUB&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0&quot;р.&quot;_-;\-* #,##0&quot;р.&quot;_-;_-* &quot;-&quot;&quot;р.&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -472,6 +500,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -746,7 +780,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -773,9 +807,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -840,6 +871,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -7603,14 +7643,14 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
     </row>
     <row r="2" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
@@ -7633,22 +7673,22 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="14">
+      <c r="A3" s="13">
         <v>20</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="14">
         <v>23</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="14">
         <v>28</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="14">
         <v>36</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="15">
         <v>39</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="16">
         <v>42</v>
       </c>
     </row>
@@ -7674,58 +7714,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="13">
+      <c r="B1" s="12">
         <v>580</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="12">
         <v>620</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="12">
         <v>870</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="12">
         <v>1300</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="12">
         <v>1400</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="12">
         <v>2220</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="12">
         <v>2900</v>
       </c>
     </row>
@@ -7740,286 +7780,286 @@
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="63" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="35" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="34" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="18"/>
-      <c r="B1" s="30"/>
+      <c r="A1" s="17"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="31"/>
+      <c r="B2" s="30"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="20"/>
-      <c r="B3" s="32"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="31"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="33"/>
+      <c r="B4" s="32"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="34">
+      <c r="B5" s="33">
         <v>1838</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="34">
+      <c r="B6" s="33">
         <v>1837</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="B7" s="33"/>
+      <c r="B7" s="32"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="34">
+      <c r="B8" s="33">
         <v>1633</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="34">
+      <c r="B9" s="33">
         <v>1632</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="22"/>
-      <c r="B10" s="31"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="30"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="31"/>
+      <c r="B11" s="30"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="20"/>
-      <c r="B12" s="32"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="31"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="B13" s="33"/>
+      <c r="B13" s="32"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="34">
+      <c r="B14" s="33">
         <v>3274</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="B15" s="33"/>
+      <c r="B15" s="32"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="B16" s="34">
+      <c r="B16" s="33">
         <v>768</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="33"/>
+      <c r="B17" s="32"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="34">
+      <c r="B18" s="33">
         <v>1263</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="34">
+      <c r="B19" s="33">
         <v>1673</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="34">
+      <c r="B20" s="33">
         <v>2423</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B21" s="34">
+      <c r="B21" s="33">
         <v>2980</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B22" s="34">
+      <c r="B22" s="33">
         <v>3738</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="B23" s="34">
+      <c r="B23" s="33">
         <v>4697</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="34">
+      <c r="B24" s="33">
         <v>5876</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="B25" s="33"/>
+      <c r="B25" s="32"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="B26" s="34">
+      <c r="B26" s="33">
         <v>1389</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="B27" s="34">
+      <c r="B27" s="33">
         <v>1886</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="B28" s="34">
+      <c r="B28" s="33">
         <v>2435</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="B29" s="34">
+      <c r="B29" s="33">
         <v>3308</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B30" s="34">
+      <c r="B30" s="33">
         <v>3367</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="B31" s="34">
+      <c r="B31" s="33">
         <v>5312</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="29" t="s">
+      <c r="A32" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="B32" s="34">
+      <c r="B32" s="33">
         <v>6397</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B33" s="33"/>
+      <c r="B33" s="32"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="B34" s="34">
+      <c r="B34" s="33">
         <v>816</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="28" t="s">
+      <c r="A35" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="B35" s="33"/>
+      <c r="B35" s="32"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="27" t="s">
+      <c r="A36" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="B36" s="34">
+      <c r="B36" s="33">
         <v>2020</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="28" t="s">
+      <c r="A37" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="B37" s="33"/>
+      <c r="B37" s="32"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="B38" s="34">
+      <c r="B38" s="33">
         <v>2414</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="29" t="s">
+      <c r="A39" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="B39" s="34">
+      <c r="B39" s="33">
         <v>3570</v>
       </c>
     </row>
@@ -8033,7 +8073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15234C30-08B1-B740-A3C1-96E9D3AD5C80}">
   <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -8044,528 +8084,712 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="37"/>
-      <c r="B1" s="42"/>
+      <c r="A1" s="36"/>
+      <c r="B1" s="41"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="43"/>
+      <c r="B2" s="42"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="38"/>
-      <c r="B3" s="44"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="43"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="39"/>
+      <c r="B4" s="38"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="B5" s="40">
+      <c r="B5" s="39">
         <v>454.55502009722426</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="40">
+      <c r="B6" s="39">
         <v>611.12397146404589</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="B7" s="40">
+      <c r="B7" s="39">
         <v>723.92095793261637</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="B8" s="40">
+      <c r="B8" s="39">
         <v>774.42707127675249</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="B9" s="40">
+      <c r="B9" s="39">
         <v>1043.7930091121445</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="B10" s="40">
+      <c r="B10" s="39">
         <v>1262.6528336034007</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="B11" s="39"/>
+      <c r="B11" s="38"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="B12" s="40">
+      <c r="B12" s="39">
         <v>420.88427786780028</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="B13" s="40">
+      <c r="B13" s="39">
         <v>276.10008628127696</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="B14" s="40">
+      <c r="B14" s="39">
         <v>732.33864348997236</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="B15" s="40">
+      <c r="B15" s="39">
         <v>791.20351859256289</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="B16" s="40">
+      <c r="B16" s="39">
         <v>622.90873124434438</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="B17" s="40">
+      <c r="B17" s="39">
         <v>816.51549906353239</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="B18" s="40">
+      <c r="B18" s="39">
         <v>969.07049987886626</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="B19" s="39"/>
+      <c r="B19" s="38"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="B20" s="40">
+      <c r="B20" s="39">
         <v>505.06113344136043</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="40">
+      <c r="B21" s="39">
         <v>707.08558681790453</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="B22" s="40">
+      <c r="B22" s="39">
         <v>824.93318462088871</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="B23" s="40">
+      <c r="B23" s="39">
         <v>826.61672173235979</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="36" t="s">
+      <c r="A24" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="B24" s="40">
+      <c r="B24" s="39">
         <v>1431.006544750521</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="B25" s="40">
+      <c r="B25" s="39">
         <v>1633.0309981270652</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="B26" s="39"/>
+      <c r="B26" s="38"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="B27" s="40">
+      <c r="B27" s="39">
         <v>368.69462741219309</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="B28" s="40">
+      <c r="B28" s="39">
         <v>456.23855720869557</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="36" t="s">
+      <c r="A29" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="B29" s="40">
+      <c r="B29" s="39">
         <v>878.8063721879671</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="B30" s="39"/>
+      <c r="B30" s="38"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="36" t="s">
+      <c r="A31" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="B31" s="40">
+      <c r="B31" s="39">
         <v>260.94825227803614</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="B32" s="40">
+      <c r="B32" s="39">
         <v>572.40261790020838</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="36" t="s">
+      <c r="A33" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="B33" s="40">
+      <c r="B33" s="39">
         <v>572.40261790020838</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="36" t="s">
+      <c r="A34" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="B34" s="40">
+      <c r="B34" s="39">
         <v>883.85698352238046</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="36" t="s">
+      <c r="A35" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="B35" s="40">
+      <c r="B35" s="39">
         <v>715.50327237526039</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="B36" s="40">
+      <c r="B36" s="39">
         <v>993.28689576800866</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="36" t="s">
+      <c r="A37" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="B37" s="40">
+      <c r="B37" s="39">
         <v>1683.5371114712011</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="28" t="s">
+      <c r="A38" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="B38" s="39"/>
+      <c r="B38" s="38"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="36" t="s">
+      <c r="A39" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="B39" s="40">
+      <c r="B39" s="39">
         <v>791.26244239146456</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="36" t="s">
+      <c r="A40" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="B40" s="40">
+      <c r="B40" s="39">
         <v>721.83029093144319</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="36" t="s">
+      <c r="A41" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="B41" s="40">
+      <c r="B41" s="39">
         <v>1341.7790778425476</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="22"/>
-      <c r="B42" s="31"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="30"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B43" s="31"/>
+      <c r="B43" s="30"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="20"/>
-      <c r="B44" s="32"/>
+      <c r="A44" s="19"/>
+      <c r="B44" s="31"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="24" t="s">
+      <c r="A45" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="B45" s="33"/>
+      <c r="B45" s="32"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="12" t="s">
+      <c r="A46" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B46" s="34">
+      <c r="B46" s="33">
         <v>3274</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="25" t="s">
+      <c r="A47" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="B47" s="33"/>
+      <c r="B47" s="32"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="26" t="s">
+      <c r="A48" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="B48" s="34">
+      <c r="B48" s="33">
         <v>768</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="24" t="s">
+      <c r="A49" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="B49" s="33"/>
+      <c r="B49" s="32"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="12" t="s">
+      <c r="A50" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B50" s="34">
+      <c r="B50" s="33">
         <v>1263</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B51" s="34">
+      <c r="B51" s="33">
         <v>1673</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="12" t="s">
+      <c r="A52" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B52" s="34">
+      <c r="B52" s="33">
         <v>2423</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="12" t="s">
+      <c r="A53" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B53" s="34">
+      <c r="B53" s="33">
         <v>2980</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="12" t="s">
+      <c r="A54" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B54" s="34">
+      <c r="B54" s="33">
         <v>3738</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="12" t="s">
+      <c r="A55" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="B55" s="34">
+      <c r="B55" s="33">
         <v>4697</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="27" t="s">
+      <c r="A56" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="B56" s="34">
+      <c r="B56" s="33">
         <v>5876</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="28" t="s">
+      <c r="A57" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="B57" s="33"/>
+      <c r="B57" s="32"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="27" t="s">
+      <c r="A58" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="B58" s="34">
+      <c r="B58" s="33">
         <v>1389</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="29" t="s">
+      <c r="A59" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="B59" s="34">
+      <c r="B59" s="33">
         <v>1886</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="29" t="s">
+      <c r="A60" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="B60" s="34">
+      <c r="B60" s="33">
         <v>2435</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="29" t="s">
+      <c r="A61" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="B61" s="34">
+      <c r="B61" s="33">
         <v>3308</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="29" t="s">
+      <c r="A62" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B62" s="34">
+      <c r="B62" s="33">
         <v>3367</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" s="29" t="s">
+      <c r="A63" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="B63" s="34">
+      <c r="B63" s="33">
         <v>5312</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" s="29" t="s">
+      <c r="A64" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="B64" s="34">
+      <c r="B64" s="33">
         <v>6397</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" s="28" t="s">
+      <c r="A65" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B65" s="33"/>
+      <c r="B65" s="32"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="27" t="s">
+      <c r="A66" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="B66" s="34">
+      <c r="B66" s="33">
         <v>816</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" s="28" t="s">
+      <c r="A67" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="B67" s="33"/>
+      <c r="B67" s="32"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="27" t="s">
+      <c r="A68" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="B68" s="34">
+      <c r="B68" s="33">
         <v>2020</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="28" t="s">
+      <c r="A69" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="B69" s="33"/>
+      <c r="B69" s="32"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="29" t="s">
+      <c r="A70" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="B70" s="34">
+      <c r="B70" s="33">
         <v>2414</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="29" t="s">
+      <c r="A71" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="B71" s="34">
+      <c r="B71" s="33">
         <v>3570</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA3EE09-DC8D-704D-9E23-A90B31F9162F}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="17"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="19"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="33">
+        <v>1838</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="33">
+        <v>1837</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="32"/>
+      <c r="C7" s="46"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="33">
+        <v>1633</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="33">
+        <v>1632</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="17"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="19"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="33">
+        <v>100</v>
+      </c>
+      <c r="C13" s="45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" s="33">
+        <v>200</v>
+      </c>
+      <c r="C14" s="45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B15" s="33">
+        <v>300</v>
+      </c>
+      <c r="C15" s="45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16" s="33">
+        <v>400</v>
+      </c>
+      <c r="C16" s="45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" s="33">
+        <v>500</v>
+      </c>
+      <c r="C17" s="45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" s="33">
+        <v>600</v>
+      </c>
+      <c r="C18" s="45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C6 C8:C9 C13:C18" xr:uid="{DEC5D86A-5307-0D4F-9BAE-93281383D310}">
+      <formula1>"Лист,Труба"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add loading side materials from excel
</commit_message>
<xml_diff>
--- a/spreadsheets/prices.xlsx
+++ b/spreadsheets/prices.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C26654-5889-7541-8DEF-353C0A7B2949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6775E48A-41F4-594E-AFCF-417C6240703A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19740" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19680" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Буквы" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="Лицевая часть" sheetId="4" r:id="rId4"/>
     <sheet name="Задник" sheetId="5" r:id="rId5"/>
     <sheet name="Каркас" sheetId="6" r:id="rId6"/>
+    <sheet name="Торец" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="132">
   <si>
     <t>Высота</t>
   </si>
@@ -871,14 +872,14 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7643,14 +7644,14 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
     </row>
     <row r="2" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
@@ -8074,7 +8075,7 @@
   <dimension ref="A1:B71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection sqref="A1:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8607,6 +8608,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -8614,7 +8616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA3EE09-DC8D-704D-9E23-A90B31F9162F}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
@@ -8655,7 +8657,7 @@
       <c r="B5" s="33">
         <v>1838</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="44" t="s">
         <v>123</v>
       </c>
     </row>
@@ -8666,7 +8668,7 @@
       <c r="B6" s="33">
         <v>1837</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="44" t="s">
         <v>123</v>
       </c>
     </row>
@@ -8675,7 +8677,7 @@
         <v>76</v>
       </c>
       <c r="B7" s="32"/>
-      <c r="C7" s="46"/>
+      <c r="C7" s="45"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
@@ -8684,7 +8686,7 @@
       <c r="B8" s="33">
         <v>1633</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="44" t="s">
         <v>123</v>
       </c>
     </row>
@@ -8695,7 +8697,7 @@
       <c r="B9" s="33">
         <v>1632</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="44" t="s">
         <v>123</v>
       </c>
     </row>
@@ -8723,7 +8725,7 @@
       <c r="B13" s="33">
         <v>100</v>
       </c>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="44" t="s">
         <v>124</v>
       </c>
     </row>
@@ -8734,7 +8736,7 @@
       <c r="B14" s="33">
         <v>200</v>
       </c>
-      <c r="C14" s="45" t="s">
+      <c r="C14" s="44" t="s">
         <v>124</v>
       </c>
     </row>
@@ -8745,7 +8747,7 @@
       <c r="B15" s="33">
         <v>300</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="44" t="s">
         <v>124</v>
       </c>
     </row>
@@ -8756,7 +8758,7 @@
       <c r="B16" s="33">
         <v>400</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="44" t="s">
         <v>124</v>
       </c>
     </row>
@@ -8767,7 +8769,7 @@
       <c r="B17" s="33">
         <v>500</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="44" t="s">
         <v>124</v>
       </c>
     </row>
@@ -8778,7 +8780,7 @@
       <c r="B18" s="33">
         <v>600</v>
       </c>
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="44" t="s">
         <v>124</v>
       </c>
     </row>
@@ -8792,4 +8794,329 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA4EEFF7-1A09-364A-8E2B-3829F5F93B3D}">
+  <dimension ref="A1:B41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="74.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="36"/>
+      <c r="B1" s="41"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="42"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="37"/>
+      <c r="B3" s="43"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="38"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="39">
+        <v>454.55502009722426</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="39">
+        <v>611.12397146404589</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="39">
+        <v>723.92095793261637</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="39">
+        <v>774.42707127675249</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" s="39">
+        <v>1043.7930091121445</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="39">
+        <v>1262.6528336034007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" s="38"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="39">
+        <v>420.88427786780028</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="39">
+        <v>276.10008628127696</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="39">
+        <v>732.33864348997236</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="39">
+        <v>791.20351859256289</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="39">
+        <v>622.90873124434438</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" s="39">
+        <v>816.51549906353239</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" s="39">
+        <v>969.07049987886626</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="38"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="39">
+        <v>505.06113344136043</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" s="39">
+        <v>707.08558681790453</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="39">
+        <v>824.93318462088871</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" s="39">
+        <v>826.61672173235979</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" s="39">
+        <v>1431.006544750521</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" s="39">
+        <v>1633.0309981270652</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" s="38"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="B27" s="39">
+        <v>368.69462741219309</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28" s="39">
+        <v>456.23855720869557</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="B29" s="39">
+        <v>878.8063721879671</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" s="38"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31" s="39">
+        <v>260.94825227803614</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" s="39">
+        <v>572.40261790020838</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" s="39">
+        <v>572.40261790020838</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" s="39">
+        <v>883.85698352238046</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" s="39">
+        <v>715.50327237526039</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="39">
+        <v>993.28689576800866</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" s="39">
+        <v>1683.5371114712011</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="B38" s="38"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" s="39">
+        <v>791.26244239146456</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" s="39">
+        <v>721.83029093144319</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" s="39">
+        <v>1341.7790778425476</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add navigation, fix letters
</commit_message>
<xml_diff>
--- a/spreadsheets/prices.xlsx
+++ b/spreadsheets/prices.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6775E48A-41F4-594E-AFCF-417C6240703A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B98EB74-B71A-234B-BC0B-83E08EA5A5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19680" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Буквы" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="134">
   <si>
     <t>Высота</t>
   </si>
@@ -432,6 +432,12 @@
   </si>
   <si>
     <t>50х50</t>
+  </si>
+  <si>
+    <t>Ы</t>
+  </si>
+  <si>
+    <t>Ъ</t>
   </si>
 </sst>
 </file>
@@ -1162,21 +1168,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:BF51"/>
+  <dimension ref="A2:BH51"/>
   <sheetViews>
-    <sheetView zoomScale="143" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="143" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB7" sqref="AB7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="28" width="5.6640625" customWidth="1"/>
-    <col min="31" max="31" width="5.5" customWidth="1"/>
-    <col min="32" max="57" width="5.6640625" customWidth="1"/>
+    <col min="2" max="30" width="5.6640625" customWidth="1"/>
+    <col min="33" max="33" width="5.5" customWidth="1"/>
+    <col min="34" max="59" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -1250,98 +1256,104 @@
         <v>26</v>
       </c>
       <c r="Y2" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AN2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="AO2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AN2" s="2" t="s">
+      <c r="AP2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AR2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AQ2" s="2" t="s">
+      <c r="AS2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AR2" s="2" t="s">
+      <c r="AT2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AS2" s="2" t="s">
+      <c r="AU2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="AT2" s="2" t="s">
+      <c r="AV2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AU2" s="2" t="s">
+      <c r="AW2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AV2" s="2" t="s">
+      <c r="AX2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AW2" s="2" t="s">
+      <c r="AY2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AX2" s="2" t="s">
+      <c r="AZ2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AY2" s="2" t="s">
+      <c r="BA2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AZ2" s="2" t="s">
+      <c r="BB2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BA2" s="5" t="s">
+      <c r="BC2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="BB2" s="2" t="s">
+      <c r="BD2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="BF2" s="6"/>
-    </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BH2" s="6"/>
+    </row>
+    <row r="3" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1418,49 +1430,49 @@
         <v>20</v>
       </c>
       <c r="Z3" s="2">
+        <v>21</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB3" s="2">
         <v>21.4</v>
       </c>
-      <c r="AA3" s="2">
+      <c r="AC3" s="2">
         <v>21</v>
-      </c>
-      <c r="AB3" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC3" s="2">
-        <v>20</v>
       </c>
       <c r="AD3" s="2">
         <v>20</v>
       </c>
       <c r="AE3" s="2">
-        <v>20.9</v>
+        <v>20</v>
       </c>
       <c r="AF3" s="2">
         <v>20</v>
       </c>
       <c r="AG3" s="2">
-        <v>20</v>
+        <v>20.9</v>
       </c>
       <c r="AH3" s="2">
         <v>20</v>
       </c>
       <c r="AI3" s="2">
-        <v>20.9</v>
+        <v>20</v>
       </c>
       <c r="AJ3" s="2">
         <v>20</v>
       </c>
       <c r="AK3" s="2">
+        <v>20.9</v>
+      </c>
+      <c r="AL3" s="2">
         <v>20</v>
-      </c>
-      <c r="AL3" s="2">
-        <v>20.399999999999999</v>
       </c>
       <c r="AM3" s="2">
         <v>20</v>
       </c>
       <c r="AN3" s="2">
-        <v>20</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="AO3" s="2">
         <v>20</v>
@@ -1469,44 +1481,50 @@
         <v>20</v>
       </c>
       <c r="AQ3" s="2">
-        <v>20.9</v>
+        <v>20</v>
       </c>
       <c r="AR3" s="2">
         <v>20</v>
       </c>
       <c r="AS3" s="2">
-        <v>22.2</v>
+        <v>20.9</v>
       </c>
       <c r="AT3" s="2">
         <v>20</v>
       </c>
       <c r="AU3" s="2">
-        <v>20.5</v>
+        <v>22.2</v>
       </c>
       <c r="AV3" s="2">
         <v>20</v>
       </c>
       <c r="AW3" s="2">
-        <v>20.399999999999999</v>
+        <v>20.5</v>
       </c>
       <c r="AX3" s="2">
         <v>20</v>
       </c>
       <c r="AY3" s="2">
-        <v>20</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="AZ3" s="2">
         <v>20</v>
       </c>
-      <c r="BA3" s="5">
+      <c r="BA3" s="2">
         <v>20</v>
       </c>
       <c r="BB3" s="2">
         <v>20</v>
       </c>
-      <c r="BF3" s="6"/>
-    </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BC3" s="5">
+        <v>20</v>
+      </c>
+      <c r="BD3" s="2">
+        <v>20</v>
+      </c>
+      <c r="BH3" s="6"/>
+    </row>
+    <row r="4" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1583,95 +1601,101 @@
         <v>18.399999999999999</v>
       </c>
       <c r="Z4" s="2">
+        <v>29.4</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="AB4" s="2">
         <v>20.8</v>
       </c>
-      <c r="AA4" s="2">
+      <c r="AC4" s="2">
         <v>29.4</v>
       </c>
-      <c r="AB4" s="2">
+      <c r="AD4" s="2">
         <v>19.600000000000001</v>
       </c>
-      <c r="AC4" s="2">
+      <c r="AE4" s="2">
         <v>21.8</v>
       </c>
-      <c r="AD4" s="2">
+      <c r="AF4" s="2">
         <v>18.5</v>
       </c>
-      <c r="AE4" s="2">
+      <c r="AG4" s="2">
         <v>19.7</v>
       </c>
-      <c r="AF4" s="2">
+      <c r="AH4" s="2">
         <v>18.399999999999999</v>
       </c>
-      <c r="AG4" s="2">
+      <c r="AI4" s="2">
         <v>16.8</v>
       </c>
-      <c r="AH4" s="2">
+      <c r="AJ4" s="2">
         <v>15.3</v>
       </c>
-      <c r="AI4" s="2">
+      <c r="AK4" s="2">
         <v>20.6</v>
       </c>
-      <c r="AJ4" s="2">
+      <c r="AL4" s="2">
         <v>19.100000000000001</v>
       </c>
-      <c r="AK4" s="2">
+      <c r="AM4" s="2">
         <v>6.2</v>
       </c>
-      <c r="AL4" s="2">
+      <c r="AN4" s="2">
         <v>16.100000000000001</v>
       </c>
-      <c r="AM4" s="2">
+      <c r="AO4" s="2">
         <v>21.2</v>
       </c>
-      <c r="AN4" s="2">
+      <c r="AP4" s="2">
         <v>15.8</v>
       </c>
-      <c r="AO4" s="2">
+      <c r="AQ4" s="2">
         <v>22.5</v>
       </c>
-      <c r="AP4" s="2">
+      <c r="AR4" s="2">
         <v>19.100000000000001</v>
       </c>
-      <c r="AQ4" s="2">
+      <c r="AS4" s="2">
         <v>20.9</v>
       </c>
-      <c r="AR4" s="2">
+      <c r="AT4" s="2">
         <v>17</v>
       </c>
-      <c r="AS4" s="2">
+      <c r="AU4" s="2">
         <v>21.1</v>
       </c>
-      <c r="AT4" s="2">
+      <c r="AV4" s="2">
         <v>19.7</v>
       </c>
-      <c r="AU4" s="2">
+      <c r="AW4" s="2">
         <v>18</v>
       </c>
-      <c r="AV4" s="2">
+      <c r="AX4" s="2">
         <v>18.8</v>
       </c>
-      <c r="AW4" s="2">
+      <c r="AY4" s="2">
         <v>19.2</v>
-      </c>
-      <c r="AX4" s="2">
-        <v>21.7</v>
-      </c>
-      <c r="AY4" s="2">
-        <v>28</v>
       </c>
       <c r="AZ4" s="2">
         <v>21.7</v>
       </c>
-      <c r="BA4" s="5">
+      <c r="BA4" s="2">
+        <v>28</v>
+      </c>
+      <c r="BB4" s="2">
         <v>21.7</v>
       </c>
-      <c r="BB4" s="2">
+      <c r="BC4" s="5">
+        <v>21.7</v>
+      </c>
+      <c r="BD4" s="2">
         <v>19</v>
       </c>
-      <c r="BF4" s="6"/>
-    </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BH4" s="6"/>
+    </row>
+    <row r="5" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1834,9 +1858,15 @@
       <c r="BB5" s="2">
         <v>6</v>
       </c>
-      <c r="BF5" s="6"/>
-    </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BC5" s="2">
+        <v>6</v>
+      </c>
+      <c r="BD5" s="2">
+        <v>6</v>
+      </c>
+      <c r="BH5" s="6"/>
+    </row>
+    <row r="6" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -1913,95 +1943,101 @@
         <v>89.6</v>
       </c>
       <c r="Z6" s="2">
+        <v>148.4</v>
+      </c>
+      <c r="AA6" s="2">
+        <v>89.6</v>
+      </c>
+      <c r="AB6" s="2">
         <v>111.5</v>
       </c>
-      <c r="AA6" s="2">
+      <c r="AC6" s="2">
         <v>148.4</v>
       </c>
-      <c r="AB6" s="2">
+      <c r="AD6" s="2">
         <v>110.5</v>
       </c>
-      <c r="AC6" s="2">
+      <c r="AE6" s="2">
         <v>95.6</v>
       </c>
-      <c r="AD6" s="2">
+      <c r="AF6" s="2">
         <v>110.1</v>
       </c>
-      <c r="AE6" s="2">
+      <c r="AG6" s="2">
         <v>97</v>
       </c>
-      <c r="AF6" s="2">
+      <c r="AH6" s="2">
         <v>100.3</v>
       </c>
-      <c r="AG6" s="2">
+      <c r="AI6" s="2">
         <v>113.7</v>
       </c>
-      <c r="AH6" s="2">
+      <c r="AJ6" s="2">
         <v>86.2</v>
       </c>
-      <c r="AI6" s="2">
+      <c r="AK6" s="2">
         <v>118</v>
       </c>
-      <c r="AJ6" s="2">
+      <c r="AL6" s="2">
         <v>108.3</v>
       </c>
-      <c r="AK6" s="2">
+      <c r="AM6" s="2">
         <v>52.4</v>
       </c>
-      <c r="AL6" s="2">
+      <c r="AN6" s="2">
         <v>71.099999999999994</v>
       </c>
-      <c r="AM6" s="2">
+      <c r="AO6" s="2">
         <v>109.7</v>
       </c>
-      <c r="AN6" s="2">
+      <c r="AP6" s="2">
         <v>71.8</v>
       </c>
-      <c r="AO6" s="2">
+      <c r="AQ6" s="2">
         <v>158.30000000000001</v>
       </c>
-      <c r="AP6" s="2">
+      <c r="AR6" s="2">
         <v>112.1</v>
       </c>
-      <c r="AQ6" s="2">
+      <c r="AS6" s="2">
         <v>100.1</v>
       </c>
-      <c r="AR6" s="2">
+      <c r="AT6" s="2">
         <v>85.5</v>
       </c>
-      <c r="AS6" s="2">
+      <c r="AU6" s="2">
         <v>112.2</v>
       </c>
-      <c r="AT6" s="2">
+      <c r="AV6" s="2">
         <v>110.7</v>
       </c>
-      <c r="AU6" s="2">
+      <c r="AW6" s="2">
         <v>107.8</v>
       </c>
-      <c r="AV6" s="2">
+      <c r="AX6" s="2">
         <v>77.7</v>
       </c>
-      <c r="AW6" s="2">
+      <c r="AY6" s="2">
         <v>101.3</v>
       </c>
-      <c r="AX6" s="2">
+      <c r="AZ6" s="2">
         <v>92.4</v>
       </c>
-      <c r="AY6" s="2">
+      <c r="BA6" s="2">
         <v>142.9</v>
       </c>
-      <c r="AZ6" s="2">
+      <c r="BB6" s="2">
         <v>104.6</v>
       </c>
-      <c r="BA6" s="5">
+      <c r="BC6" s="5">
         <v>80.400000000000006</v>
       </c>
-      <c r="BB6" s="2">
+      <c r="BD6" s="2">
         <v>107.2</v>
       </c>
-      <c r="BF6" s="6"/>
-    </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BH6" s="6"/>
+    </row>
+    <row r="7" spans="1:60" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -2029,8 +2065,8 @@
       <c r="Z7" s="3"/>
       <c r="AA7" s="3"/>
       <c r="AB7" s="3"/>
-      <c r="AF7" s="3"/>
-      <c r="AG7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
       <c r="AH7" s="3"/>
       <c r="AI7" s="3"/>
       <c r="AJ7" s="3"/>
@@ -2054,10 +2090,12 @@
       <c r="BB7" s="3"/>
       <c r="BC7" s="3"/>
       <c r="BD7" s="3"/>
-      <c r="BE7" s="6"/>
-      <c r="BF7" s="6"/>
-    </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BE7" s="3"/>
+      <c r="BF7" s="3"/>
+      <c r="BG7" s="6"/>
+      <c r="BH7" s="6"/>
+    </row>
+    <row r="8" spans="1:60" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -2085,8 +2123,8 @@
       <c r="Z8" s="3"/>
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
-      <c r="AF8" s="3"/>
-      <c r="AG8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
       <c r="AH8" s="3"/>
       <c r="AI8" s="3"/>
       <c r="AJ8" s="3"/>
@@ -2110,10 +2148,12 @@
       <c r="BB8" s="3"/>
       <c r="BC8" s="3"/>
       <c r="BD8" s="3"/>
-      <c r="BE8" s="6"/>
-      <c r="BF8" s="6"/>
-    </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BE8" s="3"/>
+      <c r="BF8" s="3"/>
+      <c r="BG8" s="6"/>
+      <c r="BH8" s="6"/>
+    </row>
+    <row r="9" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -2187,98 +2227,104 @@
         <v>26</v>
       </c>
       <c r="Y9" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z9" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Z9" s="2" t="s">
+      <c r="AB9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AA9" s="2" t="s">
+      <c r="AC9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AB9" s="2" t="s">
+      <c r="AD9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AC9" s="2" t="s">
+      <c r="AE9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AD9" s="2" t="s">
+      <c r="AF9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AE9" s="2" t="s">
+      <c r="AG9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AF9" s="2" t="s">
+      <c r="AH9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AG9" s="2" t="s">
+      <c r="AI9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AH9" s="2" t="s">
+      <c r="AJ9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AI9" s="2" t="s">
+      <c r="AK9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AJ9" s="2" t="s">
+      <c r="AL9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AK9" s="2" t="s">
+      <c r="AM9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AL9" s="2" t="s">
+      <c r="AN9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AM9" s="2" t="s">
+      <c r="AO9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AN9" s="2" t="s">
+      <c r="AP9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AO9" s="2" t="s">
+      <c r="AQ9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AP9" s="2" t="s">
+      <c r="AR9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AQ9" s="2" t="s">
+      <c r="AS9" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AR9" s="2" t="s">
+      <c r="AT9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AS9" s="2" t="s">
+      <c r="AU9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="AT9" s="2" t="s">
+      <c r="AV9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AU9" s="2" t="s">
+      <c r="AW9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AV9" s="2" t="s">
+      <c r="AX9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AW9" s="2" t="s">
+      <c r="AY9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AX9" s="2" t="s">
+      <c r="AZ9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AY9" s="2" t="s">
+      <c r="BA9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AZ9" s="2" t="s">
+      <c r="BB9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BA9" s="5" t="s">
+      <c r="BC9" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="BB9" s="2" t="s">
+      <c r="BD9" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="BF9" s="6"/>
-    </row>
-    <row r="10" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BH9" s="6"/>
+    </row>
+    <row r="10" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>0</v>
       </c>
@@ -2355,49 +2401,49 @@
         <v>40</v>
       </c>
       <c r="Z10" s="2">
+        <v>41.7</v>
+      </c>
+      <c r="AA10" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB10" s="2">
         <v>43.2</v>
       </c>
-      <c r="AA10" s="2">
+      <c r="AC10" s="2">
         <v>41.7</v>
-      </c>
-      <c r="AB10" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC10" s="2">
-        <v>40</v>
       </c>
       <c r="AD10" s="2">
         <v>40</v>
       </c>
       <c r="AE10" s="2">
-        <v>41.8</v>
+        <v>40</v>
       </c>
       <c r="AF10" s="2">
         <v>40</v>
       </c>
       <c r="AG10" s="2">
-        <v>40</v>
+        <v>41.8</v>
       </c>
       <c r="AH10" s="2">
         <v>40</v>
       </c>
       <c r="AI10" s="2">
-        <v>41.8</v>
+        <v>40</v>
       </c>
       <c r="AJ10" s="2">
         <v>40</v>
       </c>
       <c r="AK10" s="2">
+        <v>41.8</v>
+      </c>
+      <c r="AL10" s="2">
         <v>40</v>
-      </c>
-      <c r="AL10" s="2">
-        <v>40.9</v>
       </c>
       <c r="AM10" s="2">
         <v>40</v>
       </c>
       <c r="AN10" s="2">
-        <v>40</v>
+        <v>40.9</v>
       </c>
       <c r="AO10" s="2">
         <v>40</v>
@@ -2406,44 +2452,50 @@
         <v>40</v>
       </c>
       <c r="AQ10" s="2">
-        <v>41.8</v>
+        <v>40</v>
       </c>
       <c r="AR10" s="2">
         <v>40</v>
       </c>
       <c r="AS10" s="2">
-        <v>44.4</v>
+        <v>41.8</v>
       </c>
       <c r="AT10" s="2">
         <v>40</v>
       </c>
       <c r="AU10" s="2">
-        <v>41</v>
+        <v>44.4</v>
       </c>
       <c r="AV10" s="2">
         <v>40</v>
       </c>
       <c r="AW10" s="2">
-        <v>40.9</v>
+        <v>41</v>
       </c>
       <c r="AX10" s="2">
         <v>40</v>
       </c>
       <c r="AY10" s="2">
-        <v>40</v>
+        <v>40.9</v>
       </c>
       <c r="AZ10" s="2">
         <v>40</v>
       </c>
-      <c r="BA10" s="5">
+      <c r="BA10" s="2">
         <v>40</v>
       </c>
       <c r="BB10" s="2">
         <v>40</v>
       </c>
-      <c r="BF10" s="6"/>
-    </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BC10" s="5">
+        <v>40</v>
+      </c>
+      <c r="BD10" s="2">
+        <v>40</v>
+      </c>
+      <c r="BH10" s="6"/>
+    </row>
+    <row r="11" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>1</v>
       </c>
@@ -2520,95 +2572,101 @@
         <v>36.799999999999997</v>
       </c>
       <c r="Z11" s="2">
+        <v>58.4</v>
+      </c>
+      <c r="AA11" s="2">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="AB11" s="2">
         <v>41.9</v>
       </c>
-      <c r="AA11" s="2">
+      <c r="AC11" s="2">
         <v>58.4</v>
       </c>
-      <c r="AB11" s="2">
+      <c r="AD11" s="2">
         <v>39.299999999999997</v>
       </c>
-      <c r="AC11" s="2">
+      <c r="AE11" s="2">
         <v>43.6</v>
       </c>
-      <c r="AD11" s="2">
+      <c r="AF11" s="2">
         <v>37</v>
       </c>
-      <c r="AE11" s="2">
+      <c r="AG11" s="2">
         <v>39.4</v>
       </c>
-      <c r="AF11" s="2">
+      <c r="AH11" s="2">
         <v>36.799999999999997</v>
       </c>
-      <c r="AG11" s="2">
+      <c r="AI11" s="2">
         <v>33.700000000000003</v>
       </c>
-      <c r="AH11" s="2">
+      <c r="AJ11" s="2">
         <v>30.6</v>
       </c>
-      <c r="AI11" s="2">
+      <c r="AK11" s="2">
         <v>41.2</v>
       </c>
-      <c r="AJ11" s="2">
+      <c r="AL11" s="2">
         <v>38.299999999999997</v>
       </c>
-      <c r="AK11" s="2">
+      <c r="AM11" s="2">
         <v>12.4</v>
       </c>
-      <c r="AL11" s="2">
+      <c r="AN11" s="2">
         <v>32.299999999999997</v>
       </c>
-      <c r="AM11" s="2">
+      <c r="AO11" s="2">
         <v>42.4</v>
       </c>
-      <c r="AN11" s="2">
+      <c r="AP11" s="2">
         <v>31.7</v>
       </c>
-      <c r="AO11" s="2">
+      <c r="AQ11" s="2">
         <v>45</v>
       </c>
-      <c r="AP11" s="2">
+      <c r="AR11" s="2">
         <v>38.200000000000003</v>
       </c>
-      <c r="AQ11" s="2">
+      <c r="AS11" s="2">
         <v>41.9</v>
       </c>
-      <c r="AR11" s="2">
+      <c r="AT11" s="2">
         <v>34</v>
       </c>
-      <c r="AS11" s="2">
+      <c r="AU11" s="2">
         <v>42.3</v>
       </c>
-      <c r="AT11" s="2">
+      <c r="AV11" s="2">
         <v>39.4</v>
       </c>
-      <c r="AU11" s="2">
+      <c r="AW11" s="2">
         <v>36</v>
       </c>
-      <c r="AV11" s="2">
+      <c r="AX11" s="2">
         <v>37.6</v>
       </c>
-      <c r="AW11" s="2">
+      <c r="AY11" s="2">
         <v>38.5</v>
       </c>
-      <c r="AX11" s="2">
+      <c r="AZ11" s="2">
         <v>43.4</v>
       </c>
-      <c r="AY11" s="2">
+      <c r="BA11" s="2">
         <v>56</v>
       </c>
-      <c r="AZ11" s="2">
+      <c r="BB11" s="2">
         <v>43.5</v>
       </c>
-      <c r="BA11" s="5">
+      <c r="BC11" s="5">
         <v>43.5</v>
       </c>
-      <c r="BB11" s="2">
+      <c r="BD11" s="2">
         <v>38</v>
       </c>
-      <c r="BF11" s="6"/>
-    </row>
-    <row r="12" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BH11" s="6"/>
+    </row>
+    <row r="12" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>2</v>
       </c>
@@ -2771,9 +2829,15 @@
       <c r="BB12" s="2">
         <v>6</v>
       </c>
-      <c r="BF12" s="6"/>
-    </row>
-    <row r="13" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BC12" s="2">
+        <v>6</v>
+      </c>
+      <c r="BD12" s="2">
+        <v>6</v>
+      </c>
+      <c r="BH12" s="6"/>
+    </row>
+    <row r="13" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
@@ -2850,95 +2914,101 @@
         <v>179.9</v>
       </c>
       <c r="Z13" s="2">
+        <v>294.5</v>
+      </c>
+      <c r="AA13" s="2">
+        <v>179.9</v>
+      </c>
+      <c r="AB13" s="2">
         <v>224.2</v>
       </c>
-      <c r="AA13" s="2">
+      <c r="AC13" s="2">
         <v>294.5</v>
       </c>
-      <c r="AB13" s="2">
+      <c r="AD13" s="2">
         <v>221</v>
       </c>
-      <c r="AC13" s="2">
+      <c r="AE13" s="2">
         <v>191.3</v>
       </c>
-      <c r="AD13" s="2">
+      <c r="AF13" s="2">
         <v>220.3</v>
       </c>
-      <c r="AE13" s="2">
+      <c r="AG13" s="2">
         <v>194.1</v>
       </c>
-      <c r="AF13" s="2">
+      <c r="AH13" s="2">
         <v>200.7</v>
       </c>
-      <c r="AG13" s="2">
+      <c r="AI13" s="2">
         <v>227.4</v>
       </c>
-      <c r="AH13" s="2">
+      <c r="AJ13" s="2">
         <v>172.4</v>
       </c>
-      <c r="AI13" s="2">
+      <c r="AK13" s="2">
         <v>236.1</v>
       </c>
-      <c r="AJ13" s="2">
+      <c r="AL13" s="2">
         <v>217.2</v>
       </c>
-      <c r="AK13" s="2">
+      <c r="AM13" s="2">
         <v>104.9</v>
       </c>
-      <c r="AL13" s="2">
+      <c r="AN13" s="2">
         <v>142.19999999999999</v>
       </c>
-      <c r="AM13" s="2">
+      <c r="AO13" s="2">
         <v>219.4</v>
       </c>
-      <c r="AN13" s="2">
+      <c r="AP13" s="2">
         <v>143.6</v>
       </c>
-      <c r="AO13" s="2">
+      <c r="AQ13" s="2">
         <v>316.60000000000002</v>
       </c>
-      <c r="AP13" s="2">
+      <c r="AR13" s="2">
         <v>224.2</v>
       </c>
-      <c r="AQ13" s="2">
+      <c r="AS13" s="2">
         <v>200.2</v>
       </c>
-      <c r="AR13" s="2">
+      <c r="AT13" s="2">
         <v>171</v>
       </c>
-      <c r="AS13" s="2">
+      <c r="AU13" s="2">
         <v>224.5</v>
       </c>
-      <c r="AT13" s="2">
+      <c r="AV13" s="2">
         <v>221.4</v>
       </c>
-      <c r="AU13" s="2">
+      <c r="AW13" s="2">
         <v>215.6</v>
       </c>
-      <c r="AV13" s="2">
+      <c r="AX13" s="2">
         <v>155.4</v>
       </c>
-      <c r="AW13" s="2">
+      <c r="AY13" s="2">
         <v>202.7</v>
       </c>
-      <c r="AX13" s="2">
+      <c r="AZ13" s="2">
         <v>184.9</v>
       </c>
-      <c r="AY13" s="2">
+      <c r="BA13" s="2">
         <v>285.8</v>
       </c>
-      <c r="AZ13" s="2">
+      <c r="BB13" s="2">
         <v>209.2</v>
       </c>
-      <c r="BA13" s="5">
+      <c r="BC13" s="5">
         <v>160.9</v>
       </c>
-      <c r="BB13" s="2">
+      <c r="BD13" s="2">
         <v>214.4</v>
       </c>
-      <c r="BF13" s="6"/>
-    </row>
-    <row r="14" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BH13" s="6"/>
+    </row>
+    <row r="14" spans="1:60" x14ac:dyDescent="0.2">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -2966,8 +3036,8 @@
       <c r="Z14" s="3"/>
       <c r="AA14" s="3"/>
       <c r="AB14" s="3"/>
-      <c r="AF14" s="3"/>
-      <c r="AG14" s="3"/>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="3"/>
       <c r="AH14" s="3"/>
       <c r="AI14" s="3"/>
       <c r="AJ14" s="3"/>
@@ -2991,10 +3061,12 @@
       <c r="BB14" s="3"/>
       <c r="BC14" s="3"/>
       <c r="BD14" s="3"/>
-      <c r="BE14" s="6"/>
-      <c r="BF14" s="6"/>
-    </row>
-    <row r="15" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BE14" s="3"/>
+      <c r="BF14" s="3"/>
+      <c r="BG14" s="6"/>
+      <c r="BH14" s="6"/>
+    </row>
+    <row r="15" spans="1:60" x14ac:dyDescent="0.2">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -3022,8 +3094,8 @@
       <c r="Z15" s="3"/>
       <c r="AA15" s="3"/>
       <c r="AB15" s="3"/>
-      <c r="AF15" s="3"/>
-      <c r="AG15" s="3"/>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="3"/>
       <c r="AH15" s="3"/>
       <c r="AI15" s="3"/>
       <c r="AJ15" s="3"/>
@@ -3047,10 +3119,12 @@
       <c r="BB15" s="3"/>
       <c r="BC15" s="3"/>
       <c r="BD15" s="3"/>
-      <c r="BE15" s="6"/>
-      <c r="BF15" s="6"/>
-    </row>
-    <row r="16" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BE15" s="3"/>
+      <c r="BF15" s="3"/>
+      <c r="BG15" s="6"/>
+      <c r="BH15" s="6"/>
+    </row>
+    <row r="16" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
@@ -3124,98 +3198,104 @@
         <v>26</v>
       </c>
       <c r="Y16" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z16" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Z16" s="2" t="s">
+      <c r="AB16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AA16" s="2" t="s">
+      <c r="AC16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AB16" s="2" t="s">
+      <c r="AD16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AC16" s="2" t="s">
+      <c r="AE16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AD16" s="2" t="s">
+      <c r="AF16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AE16" s="2" t="s">
+      <c r="AG16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AF16" s="2" t="s">
+      <c r="AH16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AG16" s="2" t="s">
+      <c r="AI16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AH16" s="2" t="s">
+      <c r="AJ16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AI16" s="2" t="s">
+      <c r="AK16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AJ16" s="2" t="s">
+      <c r="AL16" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AK16" s="2" t="s">
+      <c r="AM16" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AL16" s="2" t="s">
+      <c r="AN16" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AM16" s="2" t="s">
+      <c r="AO16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AN16" s="2" t="s">
+      <c r="AP16" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AO16" s="2" t="s">
+      <c r="AQ16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AP16" s="2" t="s">
+      <c r="AR16" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AQ16" s="2" t="s">
+      <c r="AS16" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AR16" s="2" t="s">
+      <c r="AT16" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AS16" s="2" t="s">
+      <c r="AU16" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="AT16" s="2" t="s">
+      <c r="AV16" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AU16" s="2" t="s">
+      <c r="AW16" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AV16" s="2" t="s">
+      <c r="AX16" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AW16" s="2" t="s">
+      <c r="AY16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AX16" s="2" t="s">
+      <c r="AZ16" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AY16" s="2" t="s">
+      <c r="BA16" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AZ16" s="2" t="s">
+      <c r="BB16" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BA16" s="5" t="s">
+      <c r="BC16" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="BB16" s="2" t="s">
+      <c r="BD16" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="BF16" s="6"/>
-    </row>
-    <row r="17" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BH16" s="6"/>
+    </row>
+    <row r="17" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>0</v>
       </c>
@@ -3292,49 +3372,49 @@
         <v>60</v>
       </c>
       <c r="Z17" s="2">
+        <v>62.3</v>
+      </c>
+      <c r="AA17" s="2">
+        <v>60</v>
+      </c>
+      <c r="AB17" s="2">
         <v>63.7</v>
       </c>
-      <c r="AA17" s="2">
+      <c r="AC17" s="2">
         <v>62.3</v>
-      </c>
-      <c r="AB17" s="2">
-        <v>60</v>
-      </c>
-      <c r="AC17" s="2">
-        <v>60</v>
       </c>
       <c r="AD17" s="2">
         <v>60</v>
       </c>
       <c r="AE17" s="2">
-        <v>62.7</v>
+        <v>60</v>
       </c>
       <c r="AF17" s="2">
         <v>60</v>
       </c>
       <c r="AG17" s="2">
-        <v>60</v>
+        <v>62.7</v>
       </c>
       <c r="AH17" s="2">
         <v>60</v>
       </c>
       <c r="AI17" s="2">
-        <v>62.7</v>
+        <v>60</v>
       </c>
       <c r="AJ17" s="2">
         <v>60</v>
       </c>
       <c r="AK17" s="2">
+        <v>62.7</v>
+      </c>
+      <c r="AL17" s="2">
         <v>60</v>
-      </c>
-      <c r="AL17" s="2">
-        <v>61.2</v>
       </c>
       <c r="AM17" s="2">
         <v>60</v>
       </c>
       <c r="AN17" s="2">
-        <v>60</v>
+        <v>61.2</v>
       </c>
       <c r="AO17" s="2">
         <v>60</v>
@@ -3343,44 +3423,50 @@
         <v>60</v>
       </c>
       <c r="AQ17" s="2">
-        <v>62.7</v>
+        <v>60</v>
       </c>
       <c r="AR17" s="2">
         <v>60</v>
       </c>
       <c r="AS17" s="2">
-        <v>66.5</v>
+        <v>62.7</v>
       </c>
       <c r="AT17" s="2">
         <v>60</v>
       </c>
       <c r="AU17" s="2">
-        <v>61.4</v>
+        <v>66.5</v>
       </c>
       <c r="AV17" s="2">
         <v>60</v>
       </c>
       <c r="AW17" s="2">
-        <v>61.2</v>
+        <v>61.4</v>
       </c>
       <c r="AX17" s="2">
         <v>60</v>
       </c>
       <c r="AY17" s="2">
-        <v>60</v>
+        <v>61.2</v>
       </c>
       <c r="AZ17" s="2">
         <v>60</v>
       </c>
-      <c r="BA17" s="5">
+      <c r="BA17" s="2">
         <v>60</v>
       </c>
       <c r="BB17" s="2">
         <v>60</v>
       </c>
-      <c r="BF17" s="6"/>
-    </row>
-    <row r="18" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BC17" s="5">
+        <v>60</v>
+      </c>
+      <c r="BD17" s="2">
+        <v>60</v>
+      </c>
+      <c r="BH17" s="6"/>
+    </row>
+    <row r="18" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>1</v>
       </c>
@@ -3457,95 +3543,101 @@
         <v>55.2</v>
       </c>
       <c r="Z18" s="2">
+        <v>87.3</v>
+      </c>
+      <c r="AA18" s="2">
+        <v>55.2</v>
+      </c>
+      <c r="AB18" s="2">
         <v>61.8</v>
       </c>
-      <c r="AA18" s="2">
+      <c r="AC18" s="2">
         <v>87.3</v>
       </c>
-      <c r="AB18" s="2">
+      <c r="AD18" s="2">
         <v>58.9</v>
       </c>
-      <c r="AC18" s="2">
+      <c r="AE18" s="2">
         <v>65.3</v>
       </c>
-      <c r="AD18" s="2">
+      <c r="AF18" s="2">
         <v>55.4</v>
       </c>
-      <c r="AE18" s="2">
+      <c r="AG18" s="2">
         <v>59</v>
       </c>
-      <c r="AF18" s="2">
+      <c r="AH18" s="2">
         <v>55.2</v>
       </c>
-      <c r="AG18" s="2">
+      <c r="AI18" s="2">
         <v>50.5</v>
       </c>
-      <c r="AH18" s="2">
+      <c r="AJ18" s="2">
         <v>45.8</v>
       </c>
-      <c r="AI18" s="2">
+      <c r="AK18" s="2">
         <v>61.7</v>
       </c>
-      <c r="AJ18" s="2">
+      <c r="AL18" s="2">
         <v>57.4</v>
       </c>
-      <c r="AK18" s="2">
+      <c r="AM18" s="2">
         <v>18.600000000000001</v>
       </c>
-      <c r="AL18" s="2">
+      <c r="AN18" s="2">
         <v>48.4</v>
       </c>
-      <c r="AM18" s="2">
+      <c r="AO18" s="2">
         <v>63.6</v>
       </c>
-      <c r="AN18" s="2">
+      <c r="AP18" s="2">
         <v>47.5</v>
       </c>
-      <c r="AO18" s="2">
+      <c r="AQ18" s="2">
         <v>67.400000000000006</v>
       </c>
-      <c r="AP18" s="2">
+      <c r="AR18" s="2">
         <v>57.3</v>
       </c>
-      <c r="AQ18" s="2">
+      <c r="AS18" s="2">
         <v>62.8</v>
       </c>
-      <c r="AR18" s="2">
+      <c r="AT18" s="2">
         <v>50.9</v>
       </c>
-      <c r="AS18" s="2">
+      <c r="AU18" s="2">
         <v>63.3</v>
       </c>
-      <c r="AT18" s="2">
+      <c r="AV18" s="2">
         <v>59</v>
       </c>
-      <c r="AU18" s="2">
+      <c r="AW18" s="2">
         <v>53.9</v>
       </c>
-      <c r="AV18" s="2">
+      <c r="AX18" s="2">
         <v>56.4</v>
       </c>
-      <c r="AW18" s="2">
+      <c r="AY18" s="2">
         <v>57.7</v>
       </c>
-      <c r="AX18" s="2">
+      <c r="AZ18" s="2">
         <v>65</v>
       </c>
-      <c r="AY18" s="2">
+      <c r="BA18" s="2">
         <v>83.9</v>
       </c>
-      <c r="AZ18" s="2">
+      <c r="BB18" s="2">
         <v>65.2</v>
       </c>
-      <c r="BA18" s="5">
+      <c r="BC18" s="5">
         <v>65.3</v>
       </c>
-      <c r="BB18" s="2">
+      <c r="BD18" s="2">
         <v>56.9</v>
       </c>
-      <c r="BF18" s="6"/>
-    </row>
-    <row r="19" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BH18" s="6"/>
+    </row>
+    <row r="19" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>2</v>
       </c>
@@ -3708,9 +3800,15 @@
       <c r="BB19" s="2">
         <v>6</v>
       </c>
-      <c r="BF19" s="6"/>
-    </row>
-    <row r="20" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BC19" s="2">
+        <v>6</v>
+      </c>
+      <c r="BD19" s="2">
+        <v>6</v>
+      </c>
+      <c r="BH19" s="6"/>
+    </row>
+    <row r="20" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
@@ -3787,95 +3885,101 @@
         <v>269</v>
       </c>
       <c r="Z20" s="2">
+        <v>440</v>
+      </c>
+      <c r="AA20" s="2">
+        <v>269</v>
+      </c>
+      <c r="AB20" s="2">
         <v>330.6</v>
       </c>
-      <c r="AA20" s="2">
+      <c r="AC20" s="2">
         <v>440</v>
       </c>
-      <c r="AB20" s="2">
+      <c r="AD20" s="2">
         <v>331.5</v>
       </c>
-      <c r="AC20" s="2">
+      <c r="AE20" s="2">
         <v>286.60000000000002</v>
       </c>
-      <c r="AD20" s="2">
+      <c r="AF20" s="2">
         <v>329.9</v>
       </c>
-      <c r="AE20" s="2">
+      <c r="AG20" s="2">
         <v>290.8</v>
       </c>
-      <c r="AF20" s="2">
+      <c r="AH20" s="2">
         <v>300.60000000000002</v>
       </c>
-      <c r="AG20" s="2">
+      <c r="AI20" s="2">
         <v>340.6</v>
       </c>
-      <c r="AH20" s="2">
+      <c r="AJ20" s="2">
         <v>258.3</v>
       </c>
-      <c r="AI20" s="2">
+      <c r="AK20" s="2">
         <v>353.6</v>
       </c>
-      <c r="AJ20" s="2">
+      <c r="AL20" s="2">
         <v>325.39999999999998</v>
       </c>
-      <c r="AK20" s="2">
+      <c r="AM20" s="2">
         <v>157.19999999999999</v>
       </c>
-      <c r="AL20" s="2">
+      <c r="AN20" s="2">
         <v>213</v>
       </c>
-      <c r="AM20" s="2">
+      <c r="AO20" s="2">
         <v>328.6</v>
       </c>
-      <c r="AN20" s="2">
+      <c r="AP20" s="2">
         <v>215.1</v>
       </c>
-      <c r="AO20" s="2">
+      <c r="AQ20" s="2">
         <v>474.3</v>
       </c>
-      <c r="AP20" s="2">
+      <c r="AR20" s="2">
         <v>335.8</v>
       </c>
-      <c r="AQ20" s="2">
+      <c r="AS20" s="2">
         <v>299.8</v>
       </c>
-      <c r="AR20" s="2">
+      <c r="AT20" s="2">
         <v>256.2</v>
       </c>
-      <c r="AS20" s="2">
+      <c r="AU20" s="2">
         <v>336.3</v>
       </c>
-      <c r="AT20" s="2">
+      <c r="AV20" s="2">
         <v>331.6</v>
       </c>
-      <c r="AU20" s="2">
+      <c r="AW20" s="2">
         <v>322.89999999999998</v>
       </c>
-      <c r="AV20" s="2">
+      <c r="AX20" s="2">
         <v>232.8</v>
       </c>
-      <c r="AW20" s="2">
+      <c r="AY20" s="2">
         <v>303.60000000000002</v>
       </c>
-      <c r="AX20" s="2">
+      <c r="AZ20" s="2">
         <v>276.89999999999998</v>
       </c>
-      <c r="AY20" s="2">
+      <c r="BA20" s="2">
         <v>428.1</v>
       </c>
-      <c r="AZ20" s="2">
+      <c r="BB20" s="2">
         <v>313.39999999999998</v>
       </c>
-      <c r="BA20" s="5">
+      <c r="BC20" s="5">
         <v>241</v>
       </c>
-      <c r="BB20" s="2">
+      <c r="BD20" s="2">
         <v>321.10000000000002</v>
       </c>
-      <c r="BF20" s="6"/>
-    </row>
-    <row r="21" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BH20" s="6"/>
+    </row>
+    <row r="21" spans="1:60" x14ac:dyDescent="0.2">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -3928,10 +4032,12 @@
       <c r="AY21" s="3"/>
       <c r="AZ21" s="3"/>
       <c r="BA21" s="3"/>
-      <c r="BB21" s="6"/>
-      <c r="BF21" s="6"/>
-    </row>
-    <row r="22" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BB21" s="3"/>
+      <c r="BC21" s="3"/>
+      <c r="BD21" s="6"/>
+      <c r="BH21" s="6"/>
+    </row>
+    <row r="22" spans="1:60" x14ac:dyDescent="0.2">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -3984,10 +4090,12 @@
       <c r="AY22" s="3"/>
       <c r="AZ22" s="3"/>
       <c r="BA22" s="3"/>
-      <c r="BB22" s="6"/>
-      <c r="BF22" s="6"/>
-    </row>
-    <row r="23" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BB22" s="3"/>
+      <c r="BC22" s="3"/>
+      <c r="BD22" s="6"/>
+      <c r="BH22" s="6"/>
+    </row>
+    <row r="23" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
@@ -4061,98 +4169,104 @@
         <v>26</v>
       </c>
       <c r="Y23" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z23" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA23" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Z23" s="2" t="s">
+      <c r="AB23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AA23" s="2" t="s">
+      <c r="AC23" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AB23" s="2" t="s">
+      <c r="AD23" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AC23" s="2" t="s">
+      <c r="AE23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AD23" s="2" t="s">
+      <c r="AF23" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AE23" s="2" t="s">
+      <c r="AG23" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AF23" s="2" t="s">
+      <c r="AH23" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AG23" s="2" t="s">
+      <c r="AI23" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AH23" s="2" t="s">
+      <c r="AJ23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AI23" s="2" t="s">
+      <c r="AK23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AJ23" s="2" t="s">
+      <c r="AL23" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AK23" s="2" t="s">
+      <c r="AM23" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AL23" s="2" t="s">
+      <c r="AN23" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AM23" s="2" t="s">
+      <c r="AO23" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AN23" s="2" t="s">
+      <c r="AP23" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AO23" s="2" t="s">
+      <c r="AQ23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AP23" s="2" t="s">
+      <c r="AR23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AQ23" s="2" t="s">
+      <c r="AS23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AR23" s="2" t="s">
+      <c r="AT23" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AS23" s="2" t="s">
+      <c r="AU23" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="AT23" s="2" t="s">
+      <c r="AV23" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AU23" s="2" t="s">
+      <c r="AW23" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AV23" s="2" t="s">
+      <c r="AX23" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AW23" s="2" t="s">
+      <c r="AY23" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AX23" s="2" t="s">
+      <c r="AZ23" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AY23" s="2" t="s">
+      <c r="BA23" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AZ23" s="2" t="s">
+      <c r="BB23" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BA23" s="5" t="s">
+      <c r="BC23" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="BB23" s="2" t="s">
+      <c r="BD23" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="BF23" s="6"/>
-    </row>
-    <row r="24" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BH23" s="6"/>
+    </row>
+    <row r="24" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>0</v>
       </c>
@@ -4229,49 +4343,49 @@
         <v>80</v>
       </c>
       <c r="Z24" s="2">
+        <v>83</v>
+      </c>
+      <c r="AA24" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB24" s="2">
         <v>84</v>
       </c>
-      <c r="AA24" s="2">
+      <c r="AC24" s="2">
         <v>83</v>
-      </c>
-      <c r="AB24" s="2">
-        <v>80</v>
-      </c>
-      <c r="AC24" s="2">
-        <v>80</v>
       </c>
       <c r="AD24" s="2">
         <v>80</v>
       </c>
       <c r="AE24" s="2">
-        <v>83.6</v>
+        <v>80</v>
       </c>
       <c r="AF24" s="2">
         <v>80</v>
       </c>
       <c r="AG24" s="2">
-        <v>80</v>
+        <v>83.6</v>
       </c>
       <c r="AH24" s="2">
         <v>80</v>
       </c>
       <c r="AI24" s="2">
-        <v>83.5</v>
+        <v>80</v>
       </c>
       <c r="AJ24" s="2">
         <v>80</v>
       </c>
       <c r="AK24" s="2">
+        <v>83.5</v>
+      </c>
+      <c r="AL24" s="2">
         <v>80</v>
-      </c>
-      <c r="AL24" s="2">
-        <v>81.599999999999994</v>
       </c>
       <c r="AM24" s="2">
         <v>80</v>
       </c>
       <c r="AN24" s="2">
-        <v>80</v>
+        <v>81.599999999999994</v>
       </c>
       <c r="AO24" s="2">
         <v>80</v>
@@ -4280,44 +4394,50 @@
         <v>80</v>
       </c>
       <c r="AQ24" s="2">
-        <v>83.5</v>
+        <v>80</v>
       </c>
       <c r="AR24" s="2">
         <v>80</v>
       </c>
       <c r="AS24" s="2">
-        <v>88.7</v>
+        <v>83.5</v>
       </c>
       <c r="AT24" s="2">
         <v>80</v>
       </c>
       <c r="AU24" s="2">
-        <v>81.900000000000006</v>
+        <v>88.7</v>
       </c>
       <c r="AV24" s="2">
         <v>80</v>
       </c>
       <c r="AW24" s="2">
-        <v>81.599999999999994</v>
+        <v>81.900000000000006</v>
       </c>
       <c r="AX24" s="2">
         <v>80</v>
       </c>
       <c r="AY24" s="2">
-        <v>80</v>
+        <v>81.599999999999994</v>
       </c>
       <c r="AZ24" s="2">
         <v>80</v>
       </c>
-      <c r="BA24" s="5">
+      <c r="BA24" s="2">
         <v>80</v>
       </c>
       <c r="BB24" s="2">
         <v>80</v>
       </c>
-      <c r="BF24" s="6"/>
-    </row>
-    <row r="25" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BC24" s="5">
+        <v>80</v>
+      </c>
+      <c r="BD24" s="2">
+        <v>80</v>
+      </c>
+      <c r="BH24" s="6"/>
+    </row>
+    <row r="25" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>1</v>
       </c>
@@ -4394,95 +4514,101 @@
         <v>736</v>
       </c>
       <c r="Z25" s="2">
+        <v>116.3</v>
+      </c>
+      <c r="AA25" s="2">
+        <v>736</v>
+      </c>
+      <c r="AB25" s="2">
         <v>81.5</v>
       </c>
-      <c r="AA25" s="2">
+      <c r="AC25" s="2">
         <v>116.3</v>
       </c>
-      <c r="AB25" s="2">
+      <c r="AD25" s="2">
         <v>78.599999999999994</v>
       </c>
-      <c r="AC25" s="2">
+      <c r="AE25" s="2">
         <v>87.1</v>
       </c>
-      <c r="AD25" s="2">
+      <c r="AF25" s="2">
         <v>73.900000000000006</v>
       </c>
-      <c r="AE25" s="2">
+      <c r="AG25" s="2">
         <v>78.7</v>
       </c>
-      <c r="AF25" s="2">
+      <c r="AH25" s="2">
         <v>73.599999999999994</v>
       </c>
-      <c r="AG25" s="2">
+      <c r="AI25" s="2">
         <v>67.3</v>
       </c>
-      <c r="AH25" s="2">
+      <c r="AJ25" s="2">
         <v>61.1</v>
       </c>
-      <c r="AI25" s="2">
+      <c r="AK25" s="2">
         <v>82.3</v>
       </c>
-      <c r="AJ25" s="2">
+      <c r="AL25" s="2">
         <v>76.5</v>
       </c>
-      <c r="AK25" s="2">
+      <c r="AM25" s="2">
         <v>24.8</v>
       </c>
-      <c r="AL25" s="2">
+      <c r="AN25" s="2">
         <v>64.599999999999994</v>
       </c>
-      <c r="AM25" s="2">
+      <c r="AO25" s="2">
         <v>84.8</v>
       </c>
-      <c r="AN25" s="2">
+      <c r="AP25" s="2">
         <v>63.3</v>
       </c>
-      <c r="AO25" s="2">
+      <c r="AQ25" s="2">
         <v>89.9</v>
       </c>
-      <c r="AP25" s="2">
+      <c r="AR25" s="2">
         <v>76.400000000000006</v>
       </c>
-      <c r="AQ25" s="2">
+      <c r="AS25" s="2">
         <v>83.9</v>
       </c>
-      <c r="AR25" s="2">
+      <c r="AT25" s="2">
         <v>67.900000000000006</v>
       </c>
-      <c r="AS25" s="2">
+      <c r="AU25" s="2">
         <v>84.4</v>
       </c>
-      <c r="AT25" s="2">
+      <c r="AV25" s="2">
         <v>78.599999999999994</v>
       </c>
-      <c r="AU25" s="2">
+      <c r="AW25" s="2">
         <v>71.8</v>
       </c>
-      <c r="AV25" s="2">
+      <c r="AX25" s="2">
         <v>75.2</v>
       </c>
-      <c r="AW25" s="2">
+      <c r="AY25" s="2">
         <v>76.900000000000006</v>
       </c>
-      <c r="AX25" s="2">
+      <c r="AZ25" s="2">
         <v>86.7</v>
       </c>
-      <c r="AY25" s="2">
+      <c r="BA25" s="2">
         <v>111.8</v>
       </c>
-      <c r="AZ25" s="2">
+      <c r="BB25" s="2">
         <v>86.9</v>
       </c>
-      <c r="BA25" s="5">
+      <c r="BC25" s="5">
         <v>87</v>
       </c>
-      <c r="BB25" s="2">
+      <c r="BD25" s="2">
         <v>75.8</v>
       </c>
-      <c r="BF25" s="6"/>
-    </row>
-    <row r="26" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BH25" s="6"/>
+    </row>
+    <row r="26" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>2</v>
       </c>
@@ -4645,9 +4771,15 @@
       <c r="BB26" s="2">
         <v>8</v>
       </c>
-      <c r="BF26" s="6"/>
-    </row>
-    <row r="27" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BC26" s="2">
+        <v>8</v>
+      </c>
+      <c r="BD26" s="2">
+        <v>8</v>
+      </c>
+      <c r="BH26" s="6"/>
+    </row>
+    <row r="27" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
@@ -4724,95 +4856,101 @@
         <v>358.6</v>
       </c>
       <c r="Z27" s="2">
+        <v>586.29999999999995</v>
+      </c>
+      <c r="AA27" s="2">
+        <v>358.6</v>
+      </c>
+      <c r="AB27" s="2">
         <v>436.3</v>
       </c>
-      <c r="AA27" s="2">
+      <c r="AC27" s="2">
         <v>586.29999999999995</v>
       </c>
-      <c r="AB27" s="2">
+      <c r="AD27" s="2">
         <v>442</v>
       </c>
-      <c r="AC27" s="2">
+      <c r="AE27" s="2">
         <v>382.1</v>
       </c>
-      <c r="AD27" s="2">
+      <c r="AF27" s="2">
         <v>439.8</v>
       </c>
-      <c r="AE27" s="2">
+      <c r="AG27" s="2">
         <v>387.6</v>
       </c>
-      <c r="AF27" s="2">
+      <c r="AH27" s="2">
         <v>400.7</v>
       </c>
-      <c r="AG27" s="2">
+      <c r="AI27" s="2">
         <v>454.1</v>
       </c>
-      <c r="AH27" s="2">
+      <c r="AJ27" s="2">
         <v>344.4</v>
       </c>
-      <c r="AI27" s="2">
+      <c r="AK27" s="2">
         <v>471.4</v>
       </c>
-      <c r="AJ27" s="2">
+      <c r="AL27" s="2">
         <v>433.8</v>
       </c>
-      <c r="AK27" s="2">
+      <c r="AM27" s="2">
         <v>209.6</v>
       </c>
-      <c r="AL27" s="2">
+      <c r="AN27" s="2">
         <v>283.89999999999998</v>
       </c>
-      <c r="AM27" s="2">
+      <c r="AO27" s="2">
         <v>438.1</v>
       </c>
-      <c r="AN27" s="2">
+      <c r="AP27" s="2">
         <v>286.7</v>
       </c>
-      <c r="AO27" s="2">
+      <c r="AQ27" s="2">
         <v>632.20000000000005</v>
       </c>
-      <c r="AP27" s="2">
+      <c r="AR27" s="2">
         <v>447.6</v>
       </c>
-      <c r="AQ27" s="2">
+      <c r="AS27" s="2">
         <v>399.8</v>
       </c>
-      <c r="AR27" s="2">
+      <c r="AT27" s="2">
         <v>341.5</v>
       </c>
-      <c r="AS27" s="2">
+      <c r="AU27" s="2">
         <v>448.3</v>
       </c>
-      <c r="AT27" s="2">
+      <c r="AV27" s="2">
         <v>442.1</v>
       </c>
-      <c r="AU27" s="2">
+      <c r="AW27" s="2">
         <v>430.5</v>
       </c>
-      <c r="AV27" s="2">
+      <c r="AX27" s="2">
         <v>310.39999999999998</v>
       </c>
-      <c r="AW27" s="2">
+      <c r="AY27" s="2">
         <v>404.7</v>
       </c>
-      <c r="AX27" s="2">
+      <c r="AZ27" s="2">
         <v>369.1</v>
       </c>
-      <c r="AY27" s="2">
+      <c r="BA27" s="2">
         <v>570.70000000000005</v>
       </c>
-      <c r="AZ27" s="2">
+      <c r="BB27" s="2">
         <v>417.8</v>
       </c>
-      <c r="BA27" s="5">
+      <c r="BC27" s="5">
         <v>321.2</v>
       </c>
-      <c r="BB27" s="2">
+      <c r="BD27" s="2">
         <v>428.1</v>
       </c>
-      <c r="BF27" s="6"/>
-    </row>
-    <row r="28" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BH27" s="6"/>
+    </row>
+    <row r="28" spans="1:60" x14ac:dyDescent="0.2">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -4865,10 +5003,12 @@
       <c r="AY28" s="3"/>
       <c r="AZ28" s="3"/>
       <c r="BA28" s="3"/>
-      <c r="BB28" s="6"/>
-      <c r="BF28" s="6"/>
-    </row>
-    <row r="29" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BB28" s="3"/>
+      <c r="BC28" s="3"/>
+      <c r="BD28" s="6"/>
+      <c r="BH28" s="6"/>
+    </row>
+    <row r="29" spans="1:60" x14ac:dyDescent="0.2">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -4921,10 +5061,12 @@
       <c r="AY29" s="3"/>
       <c r="AZ29" s="3"/>
       <c r="BA29" s="3"/>
-      <c r="BB29" s="6"/>
-      <c r="BF29" s="6"/>
-    </row>
-    <row r="30" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BB29" s="3"/>
+      <c r="BC29" s="3"/>
+      <c r="BD29" s="6"/>
+      <c r="BH29" s="6"/>
+    </row>
+    <row r="30" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
@@ -4998,98 +5140,104 @@
         <v>26</v>
       </c>
       <c r="Y30" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z30" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA30" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Z30" s="2" t="s">
+      <c r="AB30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AA30" s="2" t="s">
+      <c r="AC30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AB30" s="2" t="s">
+      <c r="AD30" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AC30" s="2" t="s">
+      <c r="AE30" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AD30" s="2" t="s">
+      <c r="AF30" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AE30" s="2" t="s">
+      <c r="AG30" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AF30" s="2" t="s">
+      <c r="AH30" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AG30" s="2" t="s">
+      <c r="AI30" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AH30" s="2" t="s">
+      <c r="AJ30" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AI30" s="2" t="s">
+      <c r="AK30" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AJ30" s="2" t="s">
+      <c r="AL30" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AK30" s="2" t="s">
+      <c r="AM30" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AL30" s="2" t="s">
+      <c r="AN30" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AM30" s="2" t="s">
+      <c r="AO30" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AN30" s="2" t="s">
+      <c r="AP30" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AO30" s="2" t="s">
+      <c r="AQ30" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AP30" s="2" t="s">
+      <c r="AR30" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AQ30" s="2" t="s">
+      <c r="AS30" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AR30" s="2" t="s">
+      <c r="AT30" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AS30" s="2" t="s">
+      <c r="AU30" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="AT30" s="2" t="s">
+      <c r="AV30" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AU30" s="2" t="s">
+      <c r="AW30" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AV30" s="2" t="s">
+      <c r="AX30" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AW30" s="2" t="s">
+      <c r="AY30" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AX30" s="2" t="s">
+      <c r="AZ30" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AY30" s="2" t="s">
+      <c r="BA30" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AZ30" s="2" t="s">
+      <c r="BB30" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BA30" s="5" t="s">
+      <c r="BC30" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="BB30" s="2" t="s">
+      <c r="BD30" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="BF30" s="6"/>
-    </row>
-    <row r="31" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BH30" s="6"/>
+    </row>
+    <row r="31" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>0</v>
       </c>
@@ -5166,49 +5314,49 @@
         <v>100</v>
       </c>
       <c r="Z31" s="2">
+        <v>103.3</v>
+      </c>
+      <c r="AA31" s="2">
+        <v>100</v>
+      </c>
+      <c r="AB31" s="2">
         <v>105</v>
       </c>
-      <c r="AA31" s="2">
+      <c r="AC31" s="2">
         <v>103.3</v>
-      </c>
-      <c r="AB31" s="2">
-        <v>100</v>
-      </c>
-      <c r="AC31" s="2">
-        <v>100</v>
       </c>
       <c r="AD31" s="2">
         <v>100</v>
       </c>
       <c r="AE31" s="2">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="AF31" s="2">
         <v>100</v>
       </c>
       <c r="AG31" s="2">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="AH31" s="2">
         <v>100</v>
       </c>
       <c r="AI31" s="2">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="AJ31" s="2">
         <v>100</v>
       </c>
       <c r="AK31" s="2">
+        <v>104</v>
+      </c>
+      <c r="AL31" s="2">
         <v>100</v>
-      </c>
-      <c r="AL31" s="2">
-        <v>102</v>
       </c>
       <c r="AM31" s="2">
         <v>100</v>
       </c>
       <c r="AN31" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AO31" s="2">
         <v>100</v>
@@ -5217,44 +5365,50 @@
         <v>100</v>
       </c>
       <c r="AQ31" s="2">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="AR31" s="2">
         <v>100</v>
       </c>
       <c r="AS31" s="2">
-        <v>110.9</v>
+        <v>104</v>
       </c>
       <c r="AT31" s="2">
         <v>100</v>
       </c>
       <c r="AU31" s="2">
-        <v>102.4</v>
+        <v>110.9</v>
       </c>
       <c r="AV31" s="2">
         <v>100</v>
       </c>
       <c r="AW31" s="2">
-        <v>102</v>
+        <v>102.4</v>
       </c>
       <c r="AX31" s="2">
         <v>100</v>
       </c>
       <c r="AY31" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AZ31" s="2">
         <v>100</v>
       </c>
-      <c r="BA31" s="5">
+      <c r="BA31" s="2">
         <v>100</v>
       </c>
       <c r="BB31" s="2">
         <v>100</v>
       </c>
-      <c r="BF31" s="6"/>
-    </row>
-    <row r="32" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BC31" s="5">
+        <v>100</v>
+      </c>
+      <c r="BD31" s="2">
+        <v>100</v>
+      </c>
+      <c r="BH31" s="6"/>
+    </row>
+    <row r="32" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>1</v>
       </c>
@@ -5331,95 +5485,101 @@
         <v>92</v>
       </c>
       <c r="Z32" s="2">
+        <v>144.80000000000001</v>
+      </c>
+      <c r="AA32" s="2">
+        <v>92</v>
+      </c>
+      <c r="AB32" s="2">
         <v>101.9</v>
       </c>
-      <c r="AA32" s="2">
+      <c r="AC32" s="2">
         <v>144.80000000000001</v>
       </c>
-      <c r="AB32" s="2">
+      <c r="AD32" s="2">
         <v>98.3</v>
       </c>
-      <c r="AC32" s="2">
+      <c r="AE32" s="2">
         <v>108.9</v>
       </c>
-      <c r="AD32" s="2">
+      <c r="AF32" s="2">
         <v>92.4</v>
       </c>
-      <c r="AE32" s="2">
+      <c r="AG32" s="2">
         <v>98.4</v>
       </c>
-      <c r="AF32" s="2">
+      <c r="AH32" s="2">
         <v>92</v>
       </c>
-      <c r="AG32" s="2">
+      <c r="AI32" s="2">
         <v>84.2</v>
       </c>
-      <c r="AH32" s="2">
+      <c r="AJ32" s="2">
         <v>76.3</v>
       </c>
-      <c r="AI32" s="2">
+      <c r="AK32" s="2">
         <v>102.9</v>
       </c>
-      <c r="AJ32" s="2">
+      <c r="AL32" s="2">
         <v>95.6</v>
       </c>
-      <c r="AK32" s="2">
+      <c r="AM32" s="2">
         <v>31</v>
       </c>
-      <c r="AL32" s="2">
+      <c r="AN32" s="2">
         <v>80.7</v>
       </c>
-      <c r="AM32" s="2">
+      <c r="AO32" s="2">
         <v>106</v>
       </c>
-      <c r="AN32" s="2">
+      <c r="AP32" s="2">
         <v>79.099999999999994</v>
       </c>
-      <c r="AO32" s="2">
+      <c r="AQ32" s="2">
         <v>112.4</v>
       </c>
-      <c r="AP32" s="2">
+      <c r="AR32" s="2">
         <v>95.5</v>
       </c>
-      <c r="AQ32" s="2">
+      <c r="AS32" s="2">
         <v>104.7</v>
       </c>
-      <c r="AR32" s="2">
+      <c r="AT32" s="2">
         <v>84.9</v>
       </c>
-      <c r="AS32" s="2">
+      <c r="AU32" s="2">
         <v>105.5</v>
       </c>
-      <c r="AT32" s="2">
+      <c r="AV32" s="2">
         <v>98.3</v>
       </c>
-      <c r="AU32" s="2">
+      <c r="AW32" s="2">
         <v>89.8</v>
       </c>
-      <c r="AV32" s="2">
+      <c r="AX32" s="2">
         <v>93.9</v>
       </c>
-      <c r="AW32" s="2">
+      <c r="AY32" s="2">
         <v>96.1</v>
       </c>
-      <c r="AX32" s="2">
+      <c r="AZ32" s="2">
         <v>108.3</v>
       </c>
-      <c r="AY32" s="2">
+      <c r="BA32" s="2">
         <v>139.80000000000001</v>
       </c>
-      <c r="AZ32" s="2">
+      <c r="BB32" s="2">
         <v>108.6</v>
       </c>
-      <c r="BA32" s="5">
+      <c r="BC32" s="5">
         <v>108.8</v>
       </c>
-      <c r="BB32" s="2">
+      <c r="BD32" s="2">
         <v>94.8</v>
       </c>
-      <c r="BF32" s="6"/>
-    </row>
-    <row r="33" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BH32" s="6"/>
+    </row>
+    <row r="33" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>2</v>
       </c>
@@ -5582,9 +5742,15 @@
       <c r="BB33" s="2">
         <v>10</v>
       </c>
-      <c r="BF33" s="6"/>
-    </row>
-    <row r="34" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BC33" s="2">
+        <v>10</v>
+      </c>
+      <c r="BD33" s="2">
+        <v>10</v>
+      </c>
+      <c r="BH33" s="6"/>
+    </row>
+    <row r="34" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
@@ -5661,95 +5827,101 @@
         <v>448.3</v>
       </c>
       <c r="Z34" s="2">
+        <v>730.1</v>
+      </c>
+      <c r="AA34" s="2">
+        <v>448.3</v>
+      </c>
+      <c r="AB34" s="2">
         <v>545.20000000000005</v>
       </c>
-      <c r="AA34" s="2">
+      <c r="AC34" s="2">
         <v>730.1</v>
       </c>
-      <c r="AB34" s="2">
+      <c r="AD34" s="2">
         <v>552.5</v>
       </c>
-      <c r="AC34" s="2">
+      <c r="AE34" s="2">
         <v>477.8</v>
       </c>
-      <c r="AD34" s="2">
+      <c r="AF34" s="2">
         <v>549.70000000000005</v>
       </c>
-      <c r="AE34" s="2">
+      <c r="AG34" s="2">
         <v>484.5</v>
       </c>
-      <c r="AF34" s="2">
+      <c r="AH34" s="2">
         <v>500.9</v>
       </c>
-      <c r="AG34" s="2">
+      <c r="AI34" s="2">
         <v>567.6</v>
       </c>
-      <c r="AH34" s="2">
+      <c r="AJ34" s="2">
         <v>430.4</v>
       </c>
-      <c r="AI34" s="2">
+      <c r="AK34" s="2">
         <v>589.20000000000005</v>
       </c>
-      <c r="AJ34" s="2">
+      <c r="AL34" s="2">
         <v>542.20000000000005</v>
       </c>
-      <c r="AK34" s="2">
+      <c r="AM34" s="2">
         <v>262</v>
       </c>
-      <c r="AL34" s="2">
+      <c r="AN34" s="2">
         <v>354.9</v>
       </c>
-      <c r="AM34" s="2">
+      <c r="AO34" s="2">
         <v>547.6</v>
       </c>
-      <c r="AN34" s="2">
+      <c r="AP34" s="2">
         <v>358.3</v>
       </c>
-      <c r="AO34" s="2">
+      <c r="AQ34" s="2">
         <v>790.2</v>
       </c>
-      <c r="AP34" s="2">
+      <c r="AR34" s="2">
         <v>559.20000000000005</v>
       </c>
-      <c r="AQ34" s="2">
+      <c r="AS34" s="2">
         <v>499.7</v>
       </c>
-      <c r="AR34" s="2">
+      <c r="AT34" s="2">
         <v>426.9</v>
       </c>
-      <c r="AS34" s="2">
+      <c r="AU34" s="2">
         <v>560.29999999999995</v>
       </c>
-      <c r="AT34" s="2">
+      <c r="AV34" s="2">
         <v>552.6</v>
       </c>
-      <c r="AU34" s="2">
+      <c r="AW34" s="2">
         <v>538.1</v>
       </c>
-      <c r="AV34" s="2">
+      <c r="AX34" s="2">
         <v>388</v>
       </c>
-      <c r="AW34" s="2">
+      <c r="AY34" s="2">
         <v>505.8</v>
       </c>
-      <c r="AX34" s="2">
+      <c r="AZ34" s="2">
         <v>461.4</v>
       </c>
-      <c r="AY34" s="2">
+      <c r="BA34" s="2">
         <v>713.3</v>
       </c>
-      <c r="AZ34" s="2">
+      <c r="BB34" s="2">
         <v>522.20000000000005</v>
       </c>
-      <c r="BA34" s="5">
+      <c r="BC34" s="5">
         <v>401.5</v>
       </c>
-      <c r="BB34" s="2">
+      <c r="BD34" s="2">
         <v>535.1</v>
       </c>
-      <c r="BF34" s="6"/>
-    </row>
-    <row r="35" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BH34" s="6"/>
+    </row>
+    <row r="35" spans="1:60" x14ac:dyDescent="0.2">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -5802,10 +5974,12 @@
       <c r="AY35" s="3"/>
       <c r="AZ35" s="3"/>
       <c r="BA35" s="3"/>
-      <c r="BB35" s="6"/>
-      <c r="BF35" s="6"/>
-    </row>
-    <row r="36" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BB35" s="3"/>
+      <c r="BC35" s="3"/>
+      <c r="BD35" s="6"/>
+      <c r="BH35" s="6"/>
+    </row>
+    <row r="36" spans="1:60" x14ac:dyDescent="0.2">
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -5858,10 +6032,12 @@
       <c r="AY36" s="3"/>
       <c r="AZ36" s="3"/>
       <c r="BA36" s="3"/>
-      <c r="BB36" s="6"/>
-      <c r="BF36" s="6"/>
-    </row>
-    <row r="37" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BB36" s="3"/>
+      <c r="BC36" s="3"/>
+      <c r="BD36" s="6"/>
+      <c r="BH36" s="6"/>
+    </row>
+    <row r="37" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -5935,98 +6111,104 @@
         <v>26</v>
       </c>
       <c r="Y37" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z37" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA37" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Z37" s="2" t="s">
+      <c r="AB37" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AA37" s="2" t="s">
+      <c r="AC37" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AB37" s="2" t="s">
+      <c r="AD37" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AC37" s="2" t="s">
+      <c r="AE37" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AD37" s="2" t="s">
+      <c r="AF37" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AE37" s="2" t="s">
+      <c r="AG37" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AF37" s="2" t="s">
+      <c r="AH37" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AG37" s="2" t="s">
+      <c r="AI37" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AH37" s="2" t="s">
+      <c r="AJ37" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AI37" s="2" t="s">
+      <c r="AK37" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AJ37" s="2" t="s">
+      <c r="AL37" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AK37" s="2" t="s">
+      <c r="AM37" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AL37" s="2" t="s">
+      <c r="AN37" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AM37" s="2" t="s">
+      <c r="AO37" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AN37" s="2" t="s">
+      <c r="AP37" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AO37" s="2" t="s">
+      <c r="AQ37" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AP37" s="2" t="s">
+      <c r="AR37" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AQ37" s="2" t="s">
+      <c r="AS37" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AR37" s="2" t="s">
+      <c r="AT37" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AS37" s="2" t="s">
+      <c r="AU37" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="AT37" s="2" t="s">
+      <c r="AV37" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AU37" s="2" t="s">
+      <c r="AW37" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AV37" s="2" t="s">
+      <c r="AX37" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AW37" s="2" t="s">
+      <c r="AY37" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AX37" s="2" t="s">
+      <c r="AZ37" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AY37" s="2" t="s">
+      <c r="BA37" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AZ37" s="2" t="s">
+      <c r="BB37" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BA37" s="5" t="s">
+      <c r="BC37" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="BB37" s="2" t="s">
+      <c r="BD37" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="BF37" s="6"/>
-    </row>
-    <row r="38" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BH37" s="6"/>
+    </row>
+    <row r="38" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>0</v>
       </c>
@@ -6103,49 +6285,49 @@
         <v>120</v>
       </c>
       <c r="Z38" s="2">
+        <v>124.4</v>
+      </c>
+      <c r="AA38" s="2">
+        <v>120</v>
+      </c>
+      <c r="AB38" s="2">
         <v>125.3</v>
       </c>
-      <c r="AA38" s="2">
+      <c r="AC38" s="2">
         <v>124.4</v>
-      </c>
-      <c r="AB38" s="2">
-        <v>120</v>
-      </c>
-      <c r="AC38" s="2">
-        <v>120</v>
       </c>
       <c r="AD38" s="2">
         <v>120</v>
       </c>
       <c r="AE38" s="2">
-        <v>125.3</v>
+        <v>120</v>
       </c>
       <c r="AF38" s="2">
         <v>120</v>
       </c>
       <c r="AG38" s="2">
-        <v>120</v>
+        <v>125.3</v>
       </c>
       <c r="AH38" s="2">
         <v>120</v>
       </c>
       <c r="AI38" s="2">
-        <v>125.3</v>
+        <v>120</v>
       </c>
       <c r="AJ38" s="2">
         <v>120</v>
       </c>
       <c r="AK38" s="2">
+        <v>125.3</v>
+      </c>
+      <c r="AL38" s="2">
         <v>120</v>
-      </c>
-      <c r="AL38" s="2">
-        <v>122.4</v>
       </c>
       <c r="AM38" s="2">
         <v>120</v>
       </c>
       <c r="AN38" s="2">
-        <v>120</v>
+        <v>122.4</v>
       </c>
       <c r="AO38" s="2">
         <v>120</v>
@@ -6154,44 +6336,50 @@
         <v>120</v>
       </c>
       <c r="AQ38" s="2">
-        <v>125.3</v>
+        <v>120</v>
       </c>
       <c r="AR38" s="2">
         <v>120</v>
       </c>
       <c r="AS38" s="2">
-        <v>133.1</v>
+        <v>125.3</v>
       </c>
       <c r="AT38" s="2">
         <v>120</v>
       </c>
       <c r="AU38" s="2">
-        <v>122.9</v>
+        <v>133.1</v>
       </c>
       <c r="AV38" s="2">
         <v>120</v>
       </c>
       <c r="AW38" s="2">
-        <v>122.4</v>
+        <v>122.9</v>
       </c>
       <c r="AX38" s="2">
         <v>120</v>
       </c>
       <c r="AY38" s="2">
-        <v>120</v>
+        <v>122.4</v>
       </c>
       <c r="AZ38" s="2">
         <v>120</v>
       </c>
-      <c r="BA38" s="5">
+      <c r="BA38" s="2">
         <v>120</v>
       </c>
       <c r="BB38" s="2">
         <v>120</v>
       </c>
-      <c r="BF38" s="6"/>
-    </row>
-    <row r="39" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BC38" s="5">
+        <v>120</v>
+      </c>
+      <c r="BD38" s="2">
+        <v>120</v>
+      </c>
+      <c r="BH38" s="6"/>
+    </row>
+    <row r="39" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>1</v>
       </c>
@@ -6268,95 +6456,101 @@
         <v>110.4</v>
       </c>
       <c r="Z39" s="2">
+        <v>174.4</v>
+      </c>
+      <c r="AA39" s="2">
+        <v>110.4</v>
+      </c>
+      <c r="AB39" s="2">
         <v>129.19999999999999</v>
       </c>
-      <c r="AA39" s="2">
+      <c r="AC39" s="2">
         <v>174.4</v>
       </c>
-      <c r="AB39" s="2">
+      <c r="AD39" s="2">
         <v>117.9</v>
       </c>
-      <c r="AC39" s="2">
+      <c r="AE39" s="2">
         <v>130.69999999999999</v>
       </c>
-      <c r="AD39" s="2">
+      <c r="AF39" s="2">
         <v>110.9</v>
       </c>
-      <c r="AE39" s="2">
+      <c r="AG39" s="2">
         <v>118.1</v>
       </c>
-      <c r="AF39" s="2">
+      <c r="AH39" s="2">
         <v>110.4</v>
       </c>
-      <c r="AG39" s="2">
+      <c r="AI39" s="2">
         <v>101</v>
       </c>
-      <c r="AH39" s="2">
+      <c r="AJ39" s="2">
         <v>91.6</v>
       </c>
-      <c r="AI39" s="2">
+      <c r="AK39" s="2">
         <v>123.5</v>
       </c>
-      <c r="AJ39" s="2">
+      <c r="AL39" s="2">
         <v>114.8</v>
       </c>
-      <c r="AK39" s="2">
+      <c r="AM39" s="2">
         <v>37.200000000000003</v>
       </c>
-      <c r="AL39" s="2">
+      <c r="AN39" s="2">
         <v>96.9</v>
       </c>
-      <c r="AM39" s="2">
+      <c r="AO39" s="2">
         <v>127.2</v>
       </c>
-      <c r="AN39" s="2">
+      <c r="AP39" s="2">
         <v>95</v>
       </c>
-      <c r="AO39" s="2">
+      <c r="AQ39" s="2">
         <v>134.9</v>
       </c>
-      <c r="AP39" s="2">
+      <c r="AR39" s="2">
         <v>114.6</v>
       </c>
-      <c r="AQ39" s="2">
+      <c r="AS39" s="2">
         <v>125.7</v>
       </c>
-      <c r="AR39" s="2">
+      <c r="AT39" s="2">
         <v>101.8</v>
       </c>
-      <c r="AS39" s="2">
+      <c r="AU39" s="2">
         <v>126.7</v>
       </c>
-      <c r="AT39" s="2">
+      <c r="AV39" s="2">
         <v>117.9</v>
       </c>
-      <c r="AU39" s="2">
+      <c r="AW39" s="2">
         <v>107.8</v>
       </c>
-      <c r="AV39" s="2">
+      <c r="AX39" s="2">
         <v>112.7</v>
       </c>
-      <c r="AW39" s="2">
+      <c r="AY39" s="2">
         <v>115.4</v>
       </c>
-      <c r="AX39" s="2">
+      <c r="AZ39" s="2">
         <v>130</v>
       </c>
-      <c r="AY39" s="2">
+      <c r="BA39" s="2">
         <v>166.7</v>
       </c>
-      <c r="AZ39" s="2">
+      <c r="BB39" s="2">
         <v>130.30000000000001</v>
       </c>
-      <c r="BA39" s="5">
+      <c r="BC39" s="5">
         <v>130.5</v>
       </c>
-      <c r="BB39" s="2">
+      <c r="BD39" s="2">
         <v>113.7</v>
       </c>
-      <c r="BF39" s="6"/>
-    </row>
-    <row r="40" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BH39" s="6"/>
+    </row>
+    <row r="40" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>2</v>
       </c>
@@ -6519,9 +6713,15 @@
       <c r="BB40" s="2">
         <v>10</v>
       </c>
-      <c r="BF40" s="6"/>
-    </row>
-    <row r="41" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BC40" s="2">
+        <v>10</v>
+      </c>
+      <c r="BD40" s="2">
+        <v>10</v>
+      </c>
+      <c r="BH40" s="6"/>
+    </row>
+    <row r="41" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>3</v>
       </c>
@@ -6598,95 +6798,101 @@
         <v>538</v>
       </c>
       <c r="Z41" s="2">
+        <v>879.2</v>
+      </c>
+      <c r="AA41" s="2">
+        <v>538</v>
+      </c>
+      <c r="AB41" s="2">
         <v>670</v>
       </c>
-      <c r="AA41" s="2">
+      <c r="AC41" s="2">
         <v>879.2</v>
       </c>
-      <c r="AB41" s="2">
+      <c r="AD41" s="2">
         <v>669.1</v>
       </c>
-      <c r="AC41" s="2">
+      <c r="AE41" s="2">
         <v>573.4</v>
       </c>
-      <c r="AD41" s="2">
+      <c r="AF41" s="2">
         <v>659.7</v>
       </c>
-      <c r="AE41" s="2">
+      <c r="AG41" s="2">
         <v>581.4</v>
       </c>
-      <c r="AF41" s="2">
+      <c r="AH41" s="2">
         <v>601</v>
       </c>
-      <c r="AG41" s="2">
+      <c r="AI41" s="2">
         <v>681.1</v>
       </c>
-      <c r="AH41" s="2">
+      <c r="AJ41" s="2">
         <v>516.5</v>
       </c>
-      <c r="AI41" s="2">
+      <c r="AK41" s="2">
         <v>707</v>
       </c>
-      <c r="AJ41" s="2">
+      <c r="AL41" s="2">
         <v>650.6</v>
       </c>
-      <c r="AK41" s="2">
+      <c r="AM41" s="2">
         <v>314.39999999999998</v>
       </c>
-      <c r="AL41" s="2">
+      <c r="AN41" s="2">
         <v>425.9</v>
       </c>
-      <c r="AM41" s="2">
+      <c r="AO41" s="2">
         <v>657.1</v>
       </c>
-      <c r="AN41" s="2">
+      <c r="AP41" s="2">
         <v>430</v>
       </c>
-      <c r="AO41" s="2">
+      <c r="AQ41" s="2">
         <v>948.2</v>
       </c>
-      <c r="AP41" s="2">
+      <c r="AR41" s="2">
         <v>671.4</v>
       </c>
-      <c r="AQ41" s="2">
+      <c r="AS41" s="2">
         <v>599.70000000000005</v>
       </c>
-      <c r="AR41" s="2">
+      <c r="AT41" s="2">
         <v>512.20000000000005</v>
       </c>
-      <c r="AS41" s="2">
+      <c r="AU41" s="2">
         <v>672.3</v>
       </c>
-      <c r="AT41" s="2">
+      <c r="AV41" s="2">
         <v>633.1</v>
       </c>
-      <c r="AU41" s="2">
+      <c r="AW41" s="2">
         <v>645.6</v>
       </c>
-      <c r="AV41" s="2">
+      <c r="AX41" s="2">
         <v>465.5</v>
       </c>
-      <c r="AW41" s="2">
+      <c r="AY41" s="2">
         <v>607</v>
       </c>
-      <c r="AX41" s="2">
+      <c r="AZ41" s="2">
         <v>533.70000000000005</v>
       </c>
-      <c r="AY41" s="2">
+      <c r="BA41" s="2">
         <v>855.9</v>
       </c>
-      <c r="AZ41" s="2">
+      <c r="BB41" s="2">
         <v>626.6</v>
       </c>
-      <c r="BA41" s="5">
+      <c r="BC41" s="5">
         <v>481.8</v>
       </c>
-      <c r="BB41" s="2">
+      <c r="BD41" s="2">
         <v>642.1</v>
       </c>
-      <c r="BF41" s="6"/>
-    </row>
-    <row r="42" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BH41" s="6"/>
+    </row>
+    <row r="42" spans="1:60" x14ac:dyDescent="0.2">
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -6739,10 +6945,12 @@
       <c r="AY42" s="3"/>
       <c r="AZ42" s="3"/>
       <c r="BA42" s="3"/>
-      <c r="BB42" s="6"/>
-      <c r="BF42" s="6"/>
-    </row>
-    <row r="43" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BB42" s="3"/>
+      <c r="BC42" s="3"/>
+      <c r="BD42" s="6"/>
+      <c r="BH42" s="6"/>
+    </row>
+    <row r="43" spans="1:60" x14ac:dyDescent="0.2">
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -6795,10 +7003,12 @@
       <c r="AY43" s="3"/>
       <c r="AZ43" s="3"/>
       <c r="BA43" s="3"/>
-      <c r="BB43" s="6"/>
-      <c r="BF43" s="6"/>
-    </row>
-    <row r="44" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BB43" s="3"/>
+      <c r="BC43" s="3"/>
+      <c r="BD43" s="6"/>
+      <c r="BH43" s="6"/>
+    </row>
+    <row r="44" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>37</v>
       </c>
@@ -6872,98 +7082,104 @@
         <v>26</v>
       </c>
       <c r="Y44" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z44" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA44" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Z44" s="2" t="s">
+      <c r="AB44" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AA44" s="2" t="s">
+      <c r="AC44" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AB44" s="2" t="s">
+      <c r="AD44" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AC44" s="2" t="s">
+      <c r="AE44" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AD44" s="2" t="s">
+      <c r="AF44" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AE44" s="2" t="s">
+      <c r="AG44" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AF44" s="2" t="s">
+      <c r="AH44" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AG44" s="2" t="s">
+      <c r="AI44" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AH44" s="2" t="s">
+      <c r="AJ44" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AI44" s="2" t="s">
+      <c r="AK44" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AJ44" s="2" t="s">
+      <c r="AL44" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AK44" s="2" t="s">
+      <c r="AM44" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AL44" s="2" t="s">
+      <c r="AN44" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AM44" s="2" t="s">
+      <c r="AO44" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AN44" s="2" t="s">
+      <c r="AP44" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AO44" s="2" t="s">
+      <c r="AQ44" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AP44" s="2" t="s">
+      <c r="AR44" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AQ44" s="2" t="s">
+      <c r="AS44" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AR44" s="2" t="s">
+      <c r="AT44" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AS44" s="2" t="s">
+      <c r="AU44" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="AT44" s="2" t="s">
+      <c r="AV44" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AU44" s="2" t="s">
+      <c r="AW44" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AV44" s="2" t="s">
+      <c r="AX44" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AW44" s="2" t="s">
+      <c r="AY44" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AX44" s="2" t="s">
+      <c r="AZ44" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AY44" s="2" t="s">
+      <c r="BA44" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AZ44" s="2" t="s">
+      <c r="BB44" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BA44" s="5" t="s">
+      <c r="BC44" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="BB44" s="7" t="s">
+      <c r="BD44" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="BF44" s="6"/>
-    </row>
-    <row r="45" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BH44" s="6"/>
+    </row>
+    <row r="45" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>0</v>
       </c>
@@ -7040,49 +7256,49 @@
         <v>150</v>
       </c>
       <c r="Z45" s="2">
+        <v>152.4</v>
+      </c>
+      <c r="AA45" s="2">
         <v>150</v>
-      </c>
-      <c r="AA45" s="2">
-        <v>152.4</v>
       </c>
       <c r="AB45" s="2">
         <v>150</v>
       </c>
       <c r="AC45" s="2">
-        <v>150</v>
+        <v>152.4</v>
       </c>
       <c r="AD45" s="2">
         <v>150</v>
       </c>
       <c r="AE45" s="2">
-        <v>156.69999999999999</v>
+        <v>150</v>
       </c>
       <c r="AF45" s="2">
         <v>150</v>
       </c>
       <c r="AG45" s="2">
-        <v>150</v>
+        <v>156.69999999999999</v>
       </c>
       <c r="AH45" s="2">
         <v>150</v>
       </c>
       <c r="AI45" s="2">
-        <v>156.69999999999999</v>
+        <v>150</v>
       </c>
       <c r="AJ45" s="2">
         <v>150</v>
       </c>
       <c r="AK45" s="2">
+        <v>156.69999999999999</v>
+      </c>
+      <c r="AL45" s="2">
         <v>150</v>
-      </c>
-      <c r="AL45" s="2">
-        <v>153.1</v>
       </c>
       <c r="AM45" s="2">
         <v>150</v>
       </c>
       <c r="AN45" s="2">
-        <v>150</v>
+        <v>153.1</v>
       </c>
       <c r="AO45" s="2">
         <v>150</v>
@@ -7091,44 +7307,50 @@
         <v>150</v>
       </c>
       <c r="AQ45" s="2">
-        <v>156.69999999999999</v>
+        <v>150</v>
       </c>
       <c r="AR45" s="2">
         <v>150</v>
       </c>
       <c r="AS45" s="2">
-        <v>171.1</v>
+        <v>156.69999999999999</v>
       </c>
       <c r="AT45" s="2">
         <v>150</v>
       </c>
       <c r="AU45" s="2">
-        <v>153.6</v>
+        <v>171.1</v>
       </c>
       <c r="AV45" s="2">
         <v>150</v>
       </c>
       <c r="AW45" s="2">
-        <v>153.1</v>
+        <v>153.6</v>
       </c>
       <c r="AX45" s="2">
         <v>150</v>
       </c>
       <c r="AY45" s="2">
-        <v>150</v>
+        <v>153.1</v>
       </c>
       <c r="AZ45" s="2">
         <v>150</v>
       </c>
-      <c r="BA45" s="5">
+      <c r="BA45" s="2">
         <v>150</v>
       </c>
       <c r="BB45" s="2">
         <v>150</v>
       </c>
-      <c r="BF45" s="6"/>
-    </row>
-    <row r="46" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BC45" s="5">
+        <v>150</v>
+      </c>
+      <c r="BD45" s="2">
+        <v>150</v>
+      </c>
+      <c r="BH45" s="6"/>
+    </row>
+    <row r="46" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>1</v>
       </c>
@@ -7205,95 +7427,101 @@
         <v>138</v>
       </c>
       <c r="Z46" s="2">
+        <v>213.6</v>
+      </c>
+      <c r="AA46" s="2">
+        <v>138</v>
+      </c>
+      <c r="AB46" s="2">
         <v>145.5</v>
       </c>
-      <c r="AA46" s="2">
+      <c r="AC46" s="2">
         <v>213.6</v>
       </c>
-      <c r="AB46" s="2">
+      <c r="AD46" s="2">
         <v>147.4</v>
       </c>
-      <c r="AC46" s="2">
+      <c r="AE46" s="2">
         <v>163.4</v>
       </c>
-      <c r="AD46" s="2">
+      <c r="AF46" s="2">
         <v>138.6</v>
       </c>
-      <c r="AE46" s="2">
+      <c r="AG46" s="2">
         <v>147.6</v>
       </c>
-      <c r="AF46" s="2">
+      <c r="AH46" s="2">
         <v>138</v>
       </c>
-      <c r="AG46" s="2">
+      <c r="AI46" s="2">
         <v>126.3</v>
       </c>
-      <c r="AH46" s="2">
+      <c r="AJ46" s="2">
         <v>114.5</v>
       </c>
-      <c r="AI46" s="2">
+      <c r="AK46" s="2">
         <v>154.30000000000001</v>
       </c>
-      <c r="AJ46" s="2">
+      <c r="AL46" s="2">
         <v>143.5</v>
       </c>
-      <c r="AK46" s="2">
+      <c r="AM46" s="2">
         <v>46.5</v>
       </c>
-      <c r="AL46" s="2">
+      <c r="AN46" s="2">
         <v>121.1</v>
       </c>
-      <c r="AM46" s="2">
+      <c r="AO46" s="2">
         <v>159</v>
       </c>
-      <c r="AN46" s="2">
+      <c r="AP46" s="2">
         <v>118.7</v>
       </c>
-      <c r="AO46" s="2">
+      <c r="AQ46" s="2">
         <v>168.6</v>
       </c>
-      <c r="AP46" s="2">
+      <c r="AR46" s="2">
         <v>143.19999999999999</v>
       </c>
-      <c r="AQ46" s="2">
+      <c r="AS46" s="2">
         <v>157.1</v>
       </c>
-      <c r="AR46" s="2">
+      <c r="AT46" s="2">
         <v>127.3</v>
       </c>
-      <c r="AS46" s="2">
+      <c r="AU46" s="2">
         <v>162.80000000000001</v>
       </c>
-      <c r="AT46" s="2">
+      <c r="AV46" s="2">
         <v>147.4</v>
       </c>
-      <c r="AU46" s="2">
+      <c r="AW46" s="2">
         <v>134.69999999999999</v>
       </c>
-      <c r="AV46" s="2">
+      <c r="AX46" s="2">
         <v>140.9</v>
       </c>
-      <c r="AW46" s="2">
+      <c r="AY46" s="2">
         <v>144.19999999999999</v>
       </c>
-      <c r="AX46" s="2">
+      <c r="AZ46" s="2">
         <v>162.5</v>
       </c>
-      <c r="AY46" s="2">
+      <c r="BA46" s="2">
         <v>209.7</v>
       </c>
-      <c r="AZ46" s="2">
+      <c r="BB46" s="2">
         <v>162.9</v>
       </c>
-      <c r="BA46" s="5">
+      <c r="BC46" s="5">
         <v>163.1</v>
       </c>
-      <c r="BB46" s="2">
+      <c r="BD46" s="2">
         <v>142.19999999999999</v>
       </c>
-      <c r="BF46" s="6"/>
-    </row>
-    <row r="47" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BH46" s="6"/>
+    </row>
+    <row r="47" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>2</v>
       </c>
@@ -7456,9 +7684,15 @@
       <c r="BB47" s="2">
         <v>12</v>
       </c>
-      <c r="BF47" s="6"/>
-    </row>
-    <row r="48" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BC47" s="2">
+        <v>12</v>
+      </c>
+      <c r="BD47" s="2">
+        <v>12</v>
+      </c>
+      <c r="BH47" s="6"/>
+    </row>
+    <row r="48" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>3</v>
       </c>
@@ -7535,93 +7769,99 @@
         <v>672.5</v>
       </c>
       <c r="Z48" s="2">
+        <v>1076.9000000000001</v>
+      </c>
+      <c r="AA48" s="2">
+        <v>672.5</v>
+      </c>
+      <c r="AB48" s="2">
         <v>778.5</v>
       </c>
-      <c r="AA48" s="2">
+      <c r="AC48" s="2">
         <v>1076.9000000000001</v>
       </c>
-      <c r="AB48" s="2">
+      <c r="AD48" s="2">
         <v>828.8</v>
       </c>
-      <c r="AC48" s="2">
+      <c r="AE48" s="2">
         <v>716.7</v>
       </c>
-      <c r="AD48" s="2">
+      <c r="AF48" s="2">
         <v>824.6</v>
       </c>
-      <c r="AE48" s="2">
+      <c r="AG48" s="2">
         <v>726.7</v>
       </c>
-      <c r="AF48" s="2">
+      <c r="AH48" s="2">
         <v>751.3</v>
       </c>
-      <c r="AG48" s="2">
+      <c r="AI48" s="2">
         <v>851.3</v>
       </c>
-      <c r="AH48" s="2">
+      <c r="AJ48" s="2">
         <v>645.6</v>
       </c>
-      <c r="AI48" s="2">
+      <c r="AK48" s="2">
         <v>883.7</v>
       </c>
-      <c r="AJ48" s="2">
+      <c r="AL48" s="2">
         <v>813.2</v>
       </c>
-      <c r="AK48" s="2">
+      <c r="AM48" s="2">
         <v>393</v>
       </c>
-      <c r="AL48" s="2">
+      <c r="AN48" s="2">
         <v>532.29999999999995</v>
       </c>
-      <c r="AM48" s="2">
+      <c r="AO48" s="2">
         <v>821.3</v>
       </c>
-      <c r="AN48" s="2">
+      <c r="AP48" s="2">
         <v>537.5</v>
       </c>
-      <c r="AO48" s="2">
+      <c r="AQ48" s="2">
         <v>1185.3</v>
       </c>
-      <c r="AP48" s="2">
+      <c r="AR48" s="2">
         <v>839.2</v>
       </c>
-      <c r="AQ48" s="2">
+      <c r="AS48" s="2">
         <v>749.6</v>
       </c>
-      <c r="AR48" s="2">
+      <c r="AT48" s="2">
         <v>640.29999999999995</v>
       </c>
-      <c r="AS48" s="2">
+      <c r="AU48" s="2">
         <v>864.4</v>
       </c>
-      <c r="AT48" s="2">
+      <c r="AV48" s="2">
         <v>828.8</v>
       </c>
-      <c r="AU48" s="2">
+      <c r="AW48" s="2">
         <v>807.1</v>
       </c>
-      <c r="AV48" s="2">
+      <c r="AX48" s="2">
         <v>581.9</v>
       </c>
-      <c r="AW48" s="2">
+      <c r="AY48" s="2">
         <v>758.7</v>
       </c>
-      <c r="AX48" s="2">
+      <c r="AZ48" s="2">
         <v>692.1</v>
       </c>
-      <c r="AY48" s="2">
+      <c r="BA48" s="2">
         <v>1069.9000000000001</v>
       </c>
-      <c r="AZ48" s="2">
+      <c r="BB48" s="2">
         <v>783.2</v>
       </c>
-      <c r="BA48" s="5">
+      <c r="BC48" s="5">
         <v>602.29999999999995</v>
       </c>
-      <c r="BB48" s="2">
+      <c r="BD48" s="2">
         <v>802.6</v>
       </c>
-      <c r="BF48" s="6"/>
+      <c r="BH48" s="6"/>
     </row>
     <row r="51" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J51" s="8"/>
@@ -8800,7 +9040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA4EEFF7-1A09-364A-8E2B-3829F5F93B3D}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add light side letters
</commit_message>
<xml_diff>
--- a/spreadsheets/prices.xlsx
+++ b/spreadsheets/prices.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B98EB74-B71A-234B-BC0B-83E08EA5A5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3773DA53-C698-1647-829E-DF3C65F6FFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Буквы" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="Задник" sheetId="5" r:id="rId5"/>
     <sheet name="Каркас" sheetId="6" r:id="rId6"/>
     <sheet name="Торец" sheetId="7" r:id="rId7"/>
+    <sheet name="Световой торец" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="152">
   <si>
     <t>Высота</t>
   </si>
@@ -438,6 +439,60 @@
   </si>
   <si>
     <t>Ъ</t>
+  </si>
+  <si>
+    <t>ПОЛИСТИРОЛ ударопрочный GEBAU</t>
+  </si>
+  <si>
+    <t>ПОЛИСТИРОЛ ударопрочный (GEBAU)</t>
+  </si>
+  <si>
+    <t>1 мм белый, чёрный мат/гл (2000мм х 3000мм)</t>
+  </si>
+  <si>
+    <t>1,5 мм белый, чёрный мат/гл (2000мм х 3000мм)</t>
+  </si>
+  <si>
+    <t>2 мм белый, чёрный мат/гл (2000мм х 3000мм)</t>
+  </si>
+  <si>
+    <t>2 мм опал (КСП 35%) мат/гл (2000мм х 3000мм)</t>
+  </si>
+  <si>
+    <t>2 мм цветной мат/гл (2000мм х 3000мм)</t>
+  </si>
+  <si>
+    <t>3 мм белый, чёрный мат/гл (2000мм х 3000мм)</t>
+  </si>
+  <si>
+    <t>3 мм опал (КСП 35%) мат/гл (2000мм х 3000мм)</t>
+  </si>
+  <si>
+    <t>3 мм цветной мат/гл (2000мм х 3000мм)</t>
+  </si>
+  <si>
+    <t>4 мм белый, чёрный мат/гл (2000мм х 3000мм)</t>
+  </si>
+  <si>
+    <t>5 мм белый, чёрный мат/гл (2000мм х 3000мм)</t>
+  </si>
+  <si>
+    <t>6 мм белый, чёрный мат/гл (2000мм х 3000мм)</t>
+  </si>
+  <si>
+    <t>ПОЛИСТИРОЛ ударопрочный ЗЕРКАЛЬНЫЙ (GEBAU)</t>
+  </si>
+  <si>
+    <t>1 мм зеркальный Серебро (1000мм х 2000мм)</t>
+  </si>
+  <si>
+    <t>1 мм зеркальный Золото (1000мм х 2000мм)</t>
+  </si>
+  <si>
+    <t>2 мм зеркальный Серебро (1000мм х 2000мм)</t>
+  </si>
+  <si>
+    <t>2 мм зеркальный Золото (1000мм х 2000мм)</t>
   </si>
 </sst>
 </file>
@@ -515,7 +570,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -552,8 +607,26 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -782,12 +855,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -886,6 +990,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1170,7 +1292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:BH51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="143" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="143" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AB7" sqref="AB7"/>
     </sheetView>
   </sheetViews>
@@ -8021,7 +8143,7 @@
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B9"/>
+      <selection activeCell="A10" sqref="A10:B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9359,4 +9481,386 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F4BB0B-8E89-7E4D-BE66-74DD243F5E0B}">
+  <dimension ref="A1:B50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="21"/>
+      <c r="B1" s="30"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="30"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="19"/>
+      <c r="B3" s="31"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="32"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="33">
+        <v>3274</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="32"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="33">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="32"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="33">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="33">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="33">
+        <v>2423</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="33">
+        <v>2980</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="33">
+        <v>3738</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="33">
+        <v>4697</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="33">
+        <v>5876</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="32"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="33">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="33">
+        <v>1886</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="33">
+        <v>2435</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="33">
+        <v>3308</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="33">
+        <v>3367</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="33">
+        <v>5312</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="33">
+        <v>6397</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="32"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="33">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="32"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="33">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="32"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="33">
+        <v>2414</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="33">
+        <v>3570</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="47"/>
+      <c r="B31" s="48"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="49" t="s">
+        <v>134</v>
+      </c>
+      <c r="B32" s="50"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="51"/>
+      <c r="B33" s="52"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="53" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" s="54"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="B35" s="33">
+        <v>412.33333333333331</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="B36" s="33">
+        <v>622.80701754385962</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="B37" s="33">
+        <v>807.01754385964921</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="B38" s="33">
+        <v>828.07017543859649</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B39" s="33">
+        <v>912.28070175438597</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="B40" s="33">
+        <v>1210.5263157894738</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="B41" s="33">
+        <v>1263.1578947368423</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="B42" s="33">
+        <v>1368.421052631579</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="B43" s="33">
+        <v>1543.8596491228072</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="B44" s="33">
+        <v>2140.3508771929824</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="B45" s="33">
+        <v>2570.1754385964914</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="53" t="s">
+        <v>147</v>
+      </c>
+      <c r="B46" s="54"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="B47" s="33">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="B48" s="33">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="B49" s="33">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="B50" s="33">
+        <v>1974</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add assembly price calculator
</commit_message>
<xml_diff>
--- a/spreadsheets/prices.xlsx
+++ b/spreadsheets/prices.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3773DA53-C698-1647-829E-DF3C65F6FFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F517EC-E2D8-BB45-8089-03F4B9F595E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Буквы" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="Каркас" sheetId="6" r:id="rId6"/>
     <sheet name="Торец" sheetId="7" r:id="rId7"/>
     <sheet name="Световой торец" sheetId="8" r:id="rId8"/>
+    <sheet name="Сборка" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="153">
   <si>
     <t>Высота</t>
   </si>
@@ -493,6 +494,9 @@
   </si>
   <si>
     <t>2 мм зеркальный Золото (1000мм х 2000мм)</t>
+  </si>
+  <si>
+    <t>Цена за сборку буквы /см</t>
   </si>
 </sst>
 </file>
@@ -9487,7 +9491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F4BB0B-8E89-7E4D-BE66-74DD243F5E0B}">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -9863,4 +9867,30 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55419369-3B8D-2A47-A019-EBC713F5E7CB}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add aluminium side material
</commit_message>
<xml_diff>
--- a/spreadsheets/prices.xlsx
+++ b/spreadsheets/prices.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F517EC-E2D8-BB45-8089-03F4B9F595E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D2743B-FF1E-4D4F-9606-3A12EB3C6883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33600" yWindow="1340" windowWidth="33600" windowHeight="21000" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Буквы" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="155">
   <si>
     <t>Высота</t>
   </si>
@@ -497,6 +497,12 @@
   </si>
   <si>
     <t>Цена за сборку буквы /см</t>
+  </si>
+  <si>
+    <t>Алюминиевый борт</t>
+  </si>
+  <si>
+    <t>Полоса</t>
   </si>
 </sst>
 </file>
@@ -1296,7 +1302,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:BH51"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="143" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="143" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AB7" sqref="AB7"/>
     </sheetView>
   </sheetViews>
@@ -8440,7 +8446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15234C30-08B1-B740-A3C1-96E9D3AD5C80}">
   <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection sqref="A1:B41"/>
     </sheetView>
   </sheetViews>
@@ -9164,10 +9170,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA4EEFF7-1A09-364A-8E2B-3829F5F93B3D}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9176,314 +9182,438 @@
     <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="36"/>
       <c r="B1" s="41"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="41"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
         <v>104</v>
       </c>
       <c r="B2" s="42"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="42"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="37"/>
       <c r="B3" s="43"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="43"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
         <v>105</v>
       </c>
       <c r="B4" s="38"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="38"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="35" t="s">
         <v>107</v>
       </c>
       <c r="B5" s="39">
         <v>454.55502009722426</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="35" t="s">
         <v>108</v>
       </c>
       <c r="B6" s="39">
         <v>611.12397146404589</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="35" t="s">
         <v>109</v>
       </c>
       <c r="B7" s="39">
         <v>723.92095793261637</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="35" t="s">
         <v>110</v>
       </c>
       <c r="B8" s="39">
         <v>774.42707127675249</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="35" t="s">
         <v>111</v>
       </c>
       <c r="B9" s="39">
         <v>1043.7930091121445</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="35" t="s">
         <v>112</v>
       </c>
       <c r="B10" s="39">
         <v>1262.6528336034007</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="27" t="s">
         <v>113</v>
       </c>
       <c r="B11" s="38"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" s="38"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="35" t="s">
         <v>106</v>
       </c>
       <c r="B12" s="39">
         <v>420.88427786780028</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="35" t="s">
         <v>107</v>
       </c>
       <c r="B13" s="39">
         <v>276.10008628127696</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="35" t="s">
         <v>108</v>
       </c>
       <c r="B14" s="39">
         <v>732.33864348997236</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="35" t="s">
         <v>109</v>
       </c>
       <c r="B15" s="39">
         <v>791.20351859256289</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="35" t="s">
         <v>110</v>
       </c>
       <c r="B16" s="39">
         <v>622.90873124434438</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="35" t="s">
         <v>111</v>
       </c>
       <c r="B17" s="39">
         <v>816.51549906353239</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="35" t="s">
         <v>114</v>
       </c>
       <c r="B18" s="39">
         <v>969.07049987886626</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="27" t="s">
         <v>115</v>
       </c>
       <c r="B19" s="38"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" s="38"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="35" t="s">
         <v>107</v>
       </c>
       <c r="B20" s="39">
         <v>505.06113344136043</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="35" t="s">
         <v>108</v>
       </c>
       <c r="B21" s="39">
         <v>707.08558681790453</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="35" t="s">
         <v>109</v>
       </c>
       <c r="B22" s="39">
         <v>824.93318462088871</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="35" t="s">
         <v>110</v>
       </c>
       <c r="B23" s="39">
         <v>826.61672173235979</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="35" t="s">
         <v>111</v>
       </c>
       <c r="B24" s="39">
         <v>1431.006544750521</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="35" t="s">
         <v>112</v>
       </c>
       <c r="B25" s="39">
         <v>1633.0309981270652</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="27" t="s">
         <v>116</v>
       </c>
       <c r="B26" s="38"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26" s="38"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="35" t="s">
         <v>117</v>
       </c>
       <c r="B27" s="39">
         <v>368.69462741219309</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="35" t="s">
         <v>118</v>
       </c>
       <c r="B28" s="39">
         <v>456.23855720869557</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="35" t="s">
         <v>119</v>
       </c>
       <c r="B29" s="39">
         <v>878.8063721879671</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="40" t="s">
         <v>120</v>
       </c>
       <c r="B30" s="38"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30" s="38"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="35" t="s">
         <v>106</v>
       </c>
       <c r="B31" s="39">
         <v>260.94825227803614</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="35" t="s">
         <v>107</v>
       </c>
       <c r="B32" s="39">
         <v>572.40261790020838</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="35" t="s">
         <v>108</v>
       </c>
       <c r="B33" s="39">
         <v>572.40261790020838</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="35" t="s">
         <v>109</v>
       </c>
       <c r="B34" s="39">
         <v>883.85698352238046</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="35" t="s">
         <v>110</v>
       </c>
       <c r="B35" s="39">
         <v>715.50327237526039</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="35" t="s">
         <v>111</v>
       </c>
       <c r="B36" s="39">
         <v>993.28689576800866</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="35" t="s">
         <v>112</v>
       </c>
       <c r="B37" s="39">
         <v>1683.5371114712011</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="27" t="s">
         <v>121</v>
       </c>
       <c r="B38" s="38"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38" s="38"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="35" t="s">
         <v>107</v>
       </c>
       <c r="B39" s="39">
         <v>791.26244239146456</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="35" t="s">
         <v>122</v>
       </c>
       <c r="B40" s="39">
         <v>721.83029093144319</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="35" t="s">
         <v>109</v>
       </c>
       <c r="B41" s="39">
         <v>1341.7790778425476</v>
       </c>
+      <c r="C41" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="B43" s="35">
+        <v>24</v>
+      </c>
+      <c r="C43" s="35" t="s">
+        <v>154</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -9873,7 +10003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55419369-3B8D-2A47-A019-EBC713F5E7CB}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>